<commit_message>
rename note to memo rc
</commit_message>
<xml_diff>
--- a/db_notebook_definition.xlsx
+++ b/db_notebook_definition.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="125">
   <si>
     <t>登録日</t>
     <rPh sb="0" eb="3">
@@ -555,6 +555,30 @@
   </si>
   <si>
     <t>NN</t>
+    <phoneticPr fontId="7"/>
+  </si>
+  <si>
+    <t>memo</t>
+    <phoneticPr fontId="7"/>
+  </si>
+  <si>
+    <t>memocategory</t>
+    <phoneticPr fontId="7"/>
+  </si>
+  <si>
+    <t>memocategories</t>
+    <phoneticPr fontId="7"/>
+  </si>
+  <si>
+    <t>メモ</t>
+    <phoneticPr fontId="7"/>
+  </si>
+  <si>
+    <t>memos</t>
+    <phoneticPr fontId="7"/>
+  </si>
+  <si>
+    <t>memocategory_id</t>
     <phoneticPr fontId="7"/>
   </si>
 </sst>
@@ -827,7 +851,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -870,6 +894,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -975,7 +1005,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1133,6 +1163,60 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="33" fillId="8" borderId="5" xfId="7" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="9" borderId="0" xfId="2" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="9" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="9" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="9" borderId="5" xfId="7" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="1" xfId="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1146,7 +1230,98 @@
     <cellStyle name="標準 2" xfId="5"/>
     <cellStyle name="良い" xfId="7" builtinId="26"/>
   </cellStyles>
-  <dxfs count="78">
+  <dxfs count="91">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1703,8 +1878,8 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="テーブル133" displayName="テーブル133" ref="B6:F26" totalsRowShown="0">
   <tableColumns count="5">
-    <tableColumn id="1" name="No." dataDxfId="77"/>
-    <tableColumn id="2" name="テーブル" dataDxfId="76"/>
+    <tableColumn id="1" name="No." dataDxfId="90"/>
+    <tableColumn id="2" name="テーブル" dataDxfId="89"/>
     <tableColumn id="3" name="テーブル名"/>
     <tableColumn id="5" name="インデックス" dataCellStyle="標準 2"/>
     <tableColumn id="4" name="用途"/>
@@ -1998,10 +2173,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I126"/>
+  <dimension ref="A1:I145"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.15"/>
@@ -2555,7 +2730,7 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B34" s="42" t="s">
-        <v>103</v>
+        <v>119</v>
       </c>
       <c r="D34" s="30" t="s">
         <v>4</v>
@@ -2564,10 +2739,10 @@
         <v>5</v>
       </c>
       <c r="F34" s="31" t="s">
-        <v>90</v>
+        <v>7</v>
       </c>
       <c r="G34" s="31" t="s">
-        <v>91</v>
+        <v>8</v>
       </c>
       <c r="H34" s="32" t="s">
         <v>18</v>
@@ -2576,10 +2751,10 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B35" s="52" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="C35" s="52" t="s">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="D35" s="33"/>
       <c r="E35" s="34"/>
@@ -2588,15 +2763,15 @@
       <c r="H35" s="35"/>
       <c r="I35" s="27" t="str">
         <f xml:space="preserve"> "CREATE TABLE `" &amp; C35 &amp; "` ("</f>
-        <v>CREATE TABLE `notecategories` (</v>
+        <v>CREATE TABLE `memocategories` (</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B36" s="15" t="s">
-        <v>92</v>
+        <v>9</v>
       </c>
       <c r="C36" s="15" t="s">
-        <v>93</v>
+        <v>1</v>
       </c>
       <c r="D36" s="15" t="s">
         <v>6</v>
@@ -2608,7 +2783,7 @@
       <c r="G36" s="16"/>
       <c r="H36" s="17"/>
       <c r="I36" s="27" t="s">
-        <v>94</v>
+        <v>3</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.15">
@@ -2616,16 +2791,16 @@
         <v>15</v>
       </c>
       <c r="C37" s="15" t="s">
-        <v>95</v>
+        <v>12</v>
       </c>
       <c r="D37" s="15" t="s">
-        <v>96</v>
+        <v>13</v>
       </c>
       <c r="E37" s="16">
         <v>128</v>
       </c>
       <c r="F37" s="16" t="s">
-        <v>97</v>
+        <v>7</v>
       </c>
       <c r="G37" s="16"/>
       <c r="H37" s="17"/>
@@ -2636,17 +2811,17 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B38" s="15" t="s">
-        <v>98</v>
+        <v>36</v>
       </c>
       <c r="C38" s="15" t="s">
-        <v>98</v>
+        <v>36</v>
       </c>
       <c r="D38" s="15" t="s">
-        <v>99</v>
+        <v>16</v>
       </c>
       <c r="E38" s="16"/>
       <c r="F38" s="16" t="s">
-        <v>97</v>
+        <v>7</v>
       </c>
       <c r="G38" s="16"/>
       <c r="H38" s="17"/>
@@ -2678,7 +2853,7 @@
     <row r="40" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A40" s="22"/>
       <c r="I40" s="37" t="s">
-        <v>100</v>
+        <v>2</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.15">
@@ -2689,10 +2864,10 @@
         <v>5</v>
       </c>
       <c r="F42" s="31" t="s">
-        <v>90</v>
+        <v>7</v>
       </c>
       <c r="G42" s="31" t="s">
-        <v>91</v>
+        <v>8</v>
       </c>
       <c r="H42" s="32" t="s">
         <v>18</v>
@@ -2701,10 +2876,10 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B43" s="52" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="C43" s="52" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
       <c r="D43" s="33"/>
       <c r="E43" s="34"/>
@@ -2713,15 +2888,15 @@
       <c r="H43" s="35"/>
       <c r="I43" s="27" t="str">
         <f xml:space="preserve"> "CREATE TABLE `" &amp; C43 &amp; "` ("</f>
-        <v>CREATE TABLE `notes` (</v>
+        <v>CREATE TABLE `memos` (</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B44" s="15" t="s">
-        <v>92</v>
+        <v>9</v>
       </c>
       <c r="C44" s="15" t="s">
-        <v>93</v>
+        <v>1</v>
       </c>
       <c r="D44" s="15" t="s">
         <v>6</v>
@@ -2733,7 +2908,7 @@
       <c r="G44" s="16"/>
       <c r="H44" s="17"/>
       <c r="I44" s="27" t="s">
-        <v>94</v>
+        <v>3</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.15">
@@ -2741,10 +2916,10 @@
         <v>53</v>
       </c>
       <c r="C45" s="15" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="D45" s="15" t="s">
-        <v>104</v>
+        <v>16</v>
       </c>
       <c r="E45" s="16"/>
       <c r="F45" s="16"/>
@@ -2752,7 +2927,7 @@
       <c r="H45" s="17"/>
       <c r="I45" s="36" t="str">
         <f t="shared" ref="I45:I50" si="5">IF(A45="","","/* ") &amp; "`" &amp; C45 &amp; "` " &amp; D45 &amp; IF(E45&gt;0,"(" &amp; E45 &amp; ") "," ") &amp; IF(F45&lt;&gt;"","NOT NULL ","") &amp; IF(G45="","","DEFAULT '" &amp; G45 &amp; "' ") &amp; "COMMENT '"&amp; B45 &amp;"'," &amp; IF(A45="",""," */")</f>
-        <v>`notecategory_id` INT COMMENT '分類',</v>
+        <v>`memocategory_id` INT COMMENT '分類',</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.15">
@@ -2760,16 +2935,16 @@
         <v>15</v>
       </c>
       <c r="C46" s="15" t="s">
-        <v>95</v>
+        <v>12</v>
       </c>
       <c r="D46" s="15" t="s">
-        <v>96</v>
+        <v>13</v>
       </c>
       <c r="E46" s="16">
         <v>64</v>
       </c>
       <c r="F46" s="16" t="s">
-        <v>118</v>
+        <v>7</v>
       </c>
       <c r="G46" s="16"/>
       <c r="H46" s="17"/>
@@ -2780,13 +2955,13 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B47" s="15" t="s">
-        <v>105</v>
+        <v>45</v>
       </c>
       <c r="C47" s="15" t="s">
-        <v>106</v>
+        <v>46</v>
       </c>
       <c r="D47" s="15" t="s">
-        <v>107</v>
+        <v>17</v>
       </c>
       <c r="E47" s="16"/>
       <c r="F47" s="16"/>
@@ -2799,13 +2974,13 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B48" s="15" t="s">
-        <v>108</v>
+        <v>48</v>
       </c>
       <c r="C48" s="15" t="s">
-        <v>108</v>
+        <v>48</v>
       </c>
       <c r="D48" s="15" t="s">
-        <v>109</v>
+        <v>13</v>
       </c>
       <c r="E48" s="16">
         <v>32</v>
@@ -2820,13 +2995,13 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B49" s="15" t="s">
-        <v>110</v>
+        <v>50</v>
       </c>
       <c r="C49" s="15" t="s">
-        <v>110</v>
+        <v>50</v>
       </c>
       <c r="D49" s="15" t="s">
-        <v>109</v>
+        <v>13</v>
       </c>
       <c r="E49" s="16">
         <v>32</v>
@@ -2845,10 +3020,10 @@
         <v>0</v>
       </c>
       <c r="C50" s="18" t="s">
-        <v>111</v>
+        <v>10</v>
       </c>
       <c r="D50" s="15" t="s">
-        <v>112</v>
+        <v>11</v>
       </c>
       <c r="E50" s="16"/>
       <c r="F50" s="16"/>
@@ -2862,325 +3037,352 @@
     <row r="51" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A51" s="22"/>
       <c r="I51" s="37" t="s">
-        <v>113</v>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="B53" s="53" t="s">
+        <v>103</v>
+      </c>
+      <c r="C53" s="54"/>
+      <c r="D53" s="55" t="s">
+        <v>4</v>
+      </c>
+      <c r="E53" s="56" t="s">
+        <v>5</v>
+      </c>
+      <c r="F53" s="56" t="s">
+        <v>90</v>
+      </c>
+      <c r="G53" s="56" t="s">
+        <v>91</v>
+      </c>
+      <c r="H53" s="57" t="s">
+        <v>18</v>
+      </c>
+      <c r="I53" s="55"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="B54" s="58" t="s">
+        <v>116</v>
+      </c>
+      <c r="C54" s="58" t="s">
+        <v>101</v>
+      </c>
+      <c r="D54" s="59"/>
+      <c r="E54" s="60"/>
+      <c r="F54" s="60"/>
+      <c r="G54" s="60"/>
+      <c r="H54" s="61"/>
+      <c r="I54" s="62" t="str">
+        <f xml:space="preserve"> "CREATE TABLE `" &amp; C54 &amp; "` ("</f>
+        <v>CREATE TABLE `notecategories` (</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="B55" s="63" t="s">
+        <v>92</v>
+      </c>
+      <c r="C55" s="63" t="s">
+        <v>93</v>
+      </c>
+      <c r="D55" s="63" t="s">
+        <v>6</v>
+      </c>
+      <c r="E55" s="64" t="s">
+        <v>6</v>
+      </c>
+      <c r="F55" s="64"/>
+      <c r="G55" s="64"/>
+      <c r="H55" s="65"/>
+      <c r="I55" s="62" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="B56" s="63" t="s">
+        <v>15</v>
+      </c>
+      <c r="C56" s="63" t="s">
+        <v>95</v>
+      </c>
+      <c r="D56" s="63" t="s">
+        <v>96</v>
+      </c>
+      <c r="E56" s="64">
+        <v>128</v>
+      </c>
+      <c r="F56" s="64" t="s">
+        <v>97</v>
+      </c>
+      <c r="G56" s="64"/>
+      <c r="H56" s="65"/>
+      <c r="I56" s="66" t="str">
+        <f t="shared" ref="I56:I58" si="6">IF(A56="","","/* ") &amp; "`" &amp; C56 &amp; "` " &amp; D56 &amp; IF(E56&gt;0,"(" &amp; E56 &amp; ") "," ") &amp; IF(F56&lt;&gt;"","NOT NULL ","") &amp; IF(G56="","","DEFAULT '" &amp; G56 &amp; "' ") &amp; "COMMENT '"&amp; B56 &amp;"'," &amp; IF(A56="",""," */")</f>
+        <v>`name` VARCHAR(128) NOT NULL COMMENT '名前',</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="B57" s="63" t="s">
+        <v>98</v>
+      </c>
+      <c r="C57" s="63" t="s">
+        <v>98</v>
+      </c>
+      <c r="D57" s="63" t="s">
+        <v>99</v>
+      </c>
+      <c r="E57" s="64"/>
+      <c r="F57" s="64" t="s">
+        <v>97</v>
+      </c>
+      <c r="G57" s="64"/>
+      <c r="H57" s="65"/>
+      <c r="I57" s="66" t="str">
+        <f t="shared" si="6"/>
+        <v>`position` INT NOT NULL COMMENT 'position',</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B58" s="42" t="s">
-        <v>60</v>
-      </c>
-      <c r="D58" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="E58" s="31" t="s">
-        <v>5</v>
-      </c>
-      <c r="F58" s="31" t="s">
-        <v>7</v>
-      </c>
-      <c r="G58" s="31" t="s">
-        <v>8</v>
-      </c>
-      <c r="H58" s="32" t="s">
-        <v>18</v>
-      </c>
-      <c r="I58" s="30"/>
-    </row>
-    <row r="59" spans="1:9" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="B59" s="51" t="s">
-        <v>56</v>
-      </c>
-      <c r="C59" s="51" t="s">
-        <v>55</v>
-      </c>
-      <c r="D59" s="33"/>
-      <c r="E59" s="34"/>
-      <c r="F59" s="34"/>
-      <c r="G59" s="34"/>
-      <c r="H59" s="35"/>
-      <c r="I59" s="27" t="str">
-        <f xml:space="preserve"> "CREATE TABLE `" &amp; C59 &amp; "` ("</f>
-        <v>CREATE TABLE `todopages` (</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B60" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="C60" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="D60" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="E60" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="F60" s="16"/>
-      <c r="G60" s="16"/>
-      <c r="H60" s="17"/>
-      <c r="I60" s="27" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B61" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="C61" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="D61" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="E61" s="16">
-        <v>128</v>
-      </c>
-      <c r="F61" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="G61" s="16"/>
-      <c r="H61" s="17"/>
-      <c r="I61" s="36" t="str">
-        <f t="shared" ref="I61:I63" si="6">IF(A61="","","/* ") &amp; "`" &amp; C61 &amp; "` " &amp; D61 &amp; IF(E61&gt;0,"(" &amp; E61 &amp; ") "," ") &amp; IF(F61&lt;&gt;"","NOT NULL ","") &amp; IF(G61="","","DEFAULT '" &amp; G61 &amp; "' ") &amp; "COMMENT '"&amp; B61 &amp;"'," &amp; IF(A61="",""," */")</f>
-        <v>`name` VARCHAR(128) NOT NULL COMMENT '名前',</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B62" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="C62" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="D62" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="E62" s="16"/>
-      <c r="F62" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="G62" s="16"/>
-      <c r="H62" s="17"/>
-      <c r="I62" s="36" t="str">
-        <f t="shared" si="6"/>
-        <v>`ord` INT NOT NULL COMMENT 'ord',</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A63" s="22"/>
-      <c r="B63" s="15" t="s">
+      <c r="A58" s="22"/>
+      <c r="B58" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="C63" s="18" t="s">
+      <c r="C58" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="D63" s="15" t="s">
+      <c r="D58" s="63" t="s">
         <v>11</v>
       </c>
-      <c r="E63" s="16"/>
-      <c r="F63" s="16"/>
-      <c r="G63" s="16"/>
-      <c r="H63" s="17"/>
-      <c r="I63" s="36" t="str">
+      <c r="E58" s="64"/>
+      <c r="F58" s="64"/>
+      <c r="G58" s="64"/>
+      <c r="H58" s="65"/>
+      <c r="I58" s="66" t="str">
         <f t="shared" si="6"/>
         <v>`created` DATETIME COMMENT '登録日',</v>
       </c>
     </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A59" s="22"/>
+      <c r="B59" s="54"/>
+      <c r="C59" s="54"/>
+      <c r="D59" s="54"/>
+      <c r="E59" s="68"/>
+      <c r="F59" s="68"/>
+      <c r="G59" s="68"/>
+      <c r="H59" s="69"/>
+      <c r="I59" s="70" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="B60" s="54"/>
+      <c r="C60" s="54"/>
+      <c r="D60" s="54"/>
+      <c r="E60" s="68"/>
+      <c r="F60" s="68"/>
+      <c r="G60" s="68"/>
+      <c r="H60" s="69"/>
+      <c r="I60" s="54"/>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="B61" s="54"/>
+      <c r="C61" s="54"/>
+      <c r="D61" s="55" t="s">
+        <v>4</v>
+      </c>
+      <c r="E61" s="56" t="s">
+        <v>5</v>
+      </c>
+      <c r="F61" s="56" t="s">
+        <v>90</v>
+      </c>
+      <c r="G61" s="56" t="s">
+        <v>91</v>
+      </c>
+      <c r="H61" s="57" t="s">
+        <v>18</v>
+      </c>
+      <c r="I61" s="55"/>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="B62" s="58" t="s">
+        <v>114</v>
+      </c>
+      <c r="C62" s="58" t="s">
+        <v>115</v>
+      </c>
+      <c r="D62" s="59"/>
+      <c r="E62" s="60"/>
+      <c r="F62" s="60"/>
+      <c r="G62" s="60"/>
+      <c r="H62" s="61"/>
+      <c r="I62" s="62" t="str">
+        <f xml:space="preserve"> "CREATE TABLE `" &amp; C62 &amp; "` ("</f>
+        <v>CREATE TABLE `notes` (</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="B63" s="63" t="s">
+        <v>92</v>
+      </c>
+      <c r="C63" s="63" t="s">
+        <v>93</v>
+      </c>
+      <c r="D63" s="63" t="s">
+        <v>6</v>
+      </c>
+      <c r="E63" s="64" t="s">
+        <v>6</v>
+      </c>
+      <c r="F63" s="64"/>
+      <c r="G63" s="64"/>
+      <c r="H63" s="65"/>
+      <c r="I63" s="62" t="s">
+        <v>94</v>
+      </c>
+    </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A64" s="22"/>
-      <c r="I64" s="37" t="s">
-        <v>2</v>
+      <c r="B64" s="63" t="s">
+        <v>53</v>
+      </c>
+      <c r="C64" s="63" t="s">
+        <v>117</v>
+      </c>
+      <c r="D64" s="63" t="s">
+        <v>104</v>
+      </c>
+      <c r="E64" s="64"/>
+      <c r="F64" s="64"/>
+      <c r="G64" s="64"/>
+      <c r="H64" s="65"/>
+      <c r="I64" s="66" t="str">
+        <f t="shared" ref="I64:I69" si="7">IF(A64="","","/* ") &amp; "`" &amp; C64 &amp; "` " &amp; D64 &amp; IF(E64&gt;0,"(" &amp; E64 &amp; ") "," ") &amp; IF(F64&lt;&gt;"","NOT NULL ","") &amp; IF(G64="","","DEFAULT '" &amp; G64 &amp; "' ") &amp; "COMMENT '"&amp; B64 &amp;"'," &amp; IF(A64="",""," */")</f>
+        <v>`notecategory_id` INT COMMENT '分類',</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="B65" s="63" t="s">
+        <v>15</v>
+      </c>
+      <c r="C65" s="63" t="s">
+        <v>95</v>
+      </c>
+      <c r="D65" s="63" t="s">
+        <v>96</v>
+      </c>
+      <c r="E65" s="64">
+        <v>64</v>
+      </c>
+      <c r="F65" s="64" t="s">
+        <v>118</v>
+      </c>
+      <c r="G65" s="64"/>
+      <c r="H65" s="65"/>
+      <c r="I65" s="66" t="str">
+        <f t="shared" si="7"/>
+        <v>`name` VARCHAR(64) NOT NULL COMMENT '名前',</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="D66" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="E66" s="31" t="s">
-        <v>5</v>
-      </c>
-      <c r="F66" s="31" t="s">
-        <v>7</v>
-      </c>
-      <c r="G66" s="31" t="s">
-        <v>8</v>
-      </c>
-      <c r="H66" s="32" t="s">
-        <v>18</v>
-      </c>
-      <c r="I66" s="30"/>
-    </row>
-    <row r="67" spans="1:9" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="B67" s="51" t="s">
-        <v>34</v>
-      </c>
-      <c r="C67" s="51" t="s">
-        <v>35</v>
-      </c>
-      <c r="D67" s="33"/>
-      <c r="E67" s="34"/>
-      <c r="F67" s="34"/>
-      <c r="G67" s="34"/>
-      <c r="H67" s="35"/>
-      <c r="I67" s="27" t="str">
-        <f xml:space="preserve"> "CREATE TABLE `" &amp; C67 &amp; "` ("</f>
-        <v>CREATE TABLE `todos` (</v>
+      <c r="B66" s="63" t="s">
+        <v>105</v>
+      </c>
+      <c r="C66" s="63" t="s">
+        <v>106</v>
+      </c>
+      <c r="D66" s="63" t="s">
+        <v>107</v>
+      </c>
+      <c r="E66" s="64"/>
+      <c r="F66" s="64"/>
+      <c r="G66" s="64"/>
+      <c r="H66" s="65"/>
+      <c r="I66" s="66" t="str">
+        <f t="shared" si="7"/>
+        <v>`text` TEXT COMMENT 'テキスト',</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="B67" s="63" t="s">
+        <v>108</v>
+      </c>
+      <c r="C67" s="63" t="s">
+        <v>108</v>
+      </c>
+      <c r="D67" s="63" t="s">
+        <v>109</v>
+      </c>
+      <c r="E67" s="64">
+        <v>32</v>
+      </c>
+      <c r="F67" s="64"/>
+      <c r="G67" s="64"/>
+      <c r="H67" s="65"/>
+      <c r="I67" s="66" t="str">
+        <f t="shared" si="7"/>
+        <v>`xyz` VARCHAR(32) COMMENT 'xyz',</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B68" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="C68" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="D68" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="E68" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="F68" s="16"/>
-      <c r="G68" s="16"/>
-      <c r="H68" s="17"/>
-      <c r="I68" s="27" t="s">
-        <v>3</v>
+      <c r="B68" s="63" t="s">
+        <v>110</v>
+      </c>
+      <c r="C68" s="63" t="s">
+        <v>110</v>
+      </c>
+      <c r="D68" s="63" t="s">
+        <v>109</v>
+      </c>
+      <c r="E68" s="64">
+        <v>32</v>
+      </c>
+      <c r="F68" s="64"/>
+      <c r="G68" s="64"/>
+      <c r="H68" s="65"/>
+      <c r="I68" s="66" t="str">
+        <f t="shared" si="7"/>
+        <v>`wh` VARCHAR(32) COMMENT 'wh',</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B69" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="C69" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="D69" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="E69" s="16"/>
-      <c r="F69" s="16"/>
-      <c r="G69" s="16"/>
-      <c r="H69" s="17"/>
-      <c r="I69" s="36" t="str">
-        <f t="shared" ref="I69" si="7">IF(A69="","","/* ") &amp; "`" &amp; C69 &amp; "` " &amp; D69 &amp; IF(E69&gt;0,"(" &amp; E69 &amp; ") "," ") &amp; IF(F69&lt;&gt;"","NOT NULL ","") &amp; IF(G69="","","DEFAULT '" &amp; G69 &amp; "' ") &amp; "COMMENT '"&amp; B69 &amp;"'," &amp; IF(A69="",""," */")</f>
-        <v>`todopage_id` INT COMMENT 'page',</v>
+      <c r="A69" s="22"/>
+      <c r="B69" s="63" t="s">
+        <v>0</v>
+      </c>
+      <c r="C69" s="67" t="s">
+        <v>111</v>
+      </c>
+      <c r="D69" s="63" t="s">
+        <v>112</v>
+      </c>
+      <c r="E69" s="64"/>
+      <c r="F69" s="64"/>
+      <c r="G69" s="64"/>
+      <c r="H69" s="65"/>
+      <c r="I69" s="66" t="str">
+        <f t="shared" si="7"/>
+        <v>`created` DATETIME COMMENT '登録日',</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B70" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="C70" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="D70" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="E70" s="16"/>
-      <c r="F70" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="G70" s="16"/>
-      <c r="H70" s="17"/>
-      <c r="I70" s="36" t="str">
-        <f t="shared" ref="I70" si="8">IF(A70="","","/* ") &amp; "`" &amp; C70 &amp; "` " &amp; D70 &amp; IF(E70&gt;0,"(" &amp; E70 &amp; ") "," ") &amp; IF(F70&lt;&gt;"","NOT NULL ","") &amp; IF(G70="","","DEFAULT '" &amp; G70 &amp; "' ") &amp; "COMMENT '"&amp; B70 &amp;"'," &amp; IF(A70="",""," */")</f>
-        <v>`position` INT NOT NULL COMMENT 'position',</v>
-      </c>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B71" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="C71" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="D71" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="E71" s="16">
-        <v>128</v>
-      </c>
-      <c r="F71" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="G71" s="16"/>
-      <c r="H71" s="17"/>
-      <c r="I71" s="36" t="str">
-        <f t="shared" ref="I71:I74" si="9">IF(A71="","","/* ") &amp; "`" &amp; C71 &amp; "` " &amp; D71 &amp; IF(E71&gt;0,"(" &amp; E71 &amp; ") "," ") &amp; IF(F71&lt;&gt;"","NOT NULL ","") &amp; IF(G71="","","DEFAULT '" &amp; G71 &amp; "' ") &amp; "COMMENT '"&amp; B71 &amp;"'," &amp; IF(A71="",""," */")</f>
-        <v>`name` VARCHAR(128) NOT NULL COMMENT '名前',</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B72" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="C72" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="D72" s="15" t="s">
-        <v>77</v>
-      </c>
-      <c r="E72" s="16"/>
-      <c r="F72" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="G72" s="16">
-        <v>0</v>
-      </c>
-      <c r="H72" s="17"/>
-      <c r="I72" s="36" t="str">
-        <f t="shared" si="9"/>
-        <v>`emphasis` BOOLEAN NOT NULL DEFAULT '0' COMMENT 'emphasis',</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A73" s="22"/>
-      <c r="B73" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="C73" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="D73" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="E73" s="16"/>
-      <c r="F73" s="16"/>
-      <c r="G73" s="16"/>
-      <c r="H73" s="17"/>
-      <c r="I73" s="36" t="str">
-        <f t="shared" si="9"/>
-        <v>`created` DATETIME COMMENT '登録日',</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A74" s="22"/>
-      <c r="B74" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="C74" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="D74" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="E74" s="16"/>
-      <c r="F74" s="16"/>
-      <c r="G74" s="16"/>
-      <c r="H74" s="17"/>
-      <c r="I74" s="36" t="str">
-        <f t="shared" si="9"/>
-        <v>`completed` DATE COMMENT '完了日',</v>
-      </c>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A75" s="22"/>
-      <c r="I75" s="37" t="s">
-        <v>2</v>
+      <c r="A70" s="22"/>
+      <c r="B70" s="54"/>
+      <c r="C70" s="54"/>
+      <c r="D70" s="54"/>
+      <c r="E70" s="68"/>
+      <c r="F70" s="68"/>
+      <c r="G70" s="68"/>
+      <c r="H70" s="69"/>
+      <c r="I70" s="70" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="B77" s="42" t="s">
+        <v>60</v>
+      </c>
       <c r="D77" s="30" t="s">
         <v>4</v>
       </c>
@@ -3200,10 +3402,10 @@
     </row>
     <row r="78" spans="1:9" ht="16.5" x14ac:dyDescent="0.15">
       <c r="B78" s="51" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="C78" s="51" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="D78" s="33"/>
       <c r="E78" s="34"/>
@@ -3212,7 +3414,7 @@
       <c r="H78" s="35"/>
       <c r="I78" s="27" t="str">
         <f xml:space="preserve"> "CREATE TABLE `" &amp; C78 &amp; "` ("</f>
-        <v>CREATE TABLE `histories` (</v>
+        <v>CREATE TABLE `todopages` (</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.15">
@@ -3237,768 +3439,769 @@
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B80" s="15" t="s">
-        <v>54</v>
+        <v>15</v>
       </c>
       <c r="C80" s="15" t="s">
-        <v>58</v>
+        <v>12</v>
       </c>
       <c r="D80" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="E80" s="16"/>
-      <c r="F80" s="16"/>
+        <v>13</v>
+      </c>
+      <c r="E80" s="16">
+        <v>128</v>
+      </c>
+      <c r="F80" s="16" t="s">
+        <v>7</v>
+      </c>
       <c r="G80" s="16"/>
       <c r="H80" s="17"/>
       <c r="I80" s="36" t="str">
-        <f t="shared" ref="I80" si="10">IF(A80="","","/* ") &amp; "`" &amp; C80 &amp; "` " &amp; D80 &amp; IF(E80&gt;0,"(" &amp; E80 &amp; ") "," ") &amp; IF(F80&lt;&gt;"","NOT NULL ","") &amp; IF(G80="","","DEFAULT '" &amp; G80 &amp; "' ") &amp; "COMMENT '"&amp; B80 &amp;"'," &amp; IF(A80="",""," */")</f>
-        <v>`pageid` INT COMMENT 'page',</v>
+        <f t="shared" ref="I80:I82" si="8">IF(A80="","","/* ") &amp; "`" &amp; C80 &amp; "` " &amp; D80 &amp; IF(E80&gt;0,"(" &amp; E80 &amp; ") "," ") &amp; IF(F80&lt;&gt;"","NOT NULL ","") &amp; IF(G80="","","DEFAULT '" &amp; G80 &amp; "' ") &amp; "COMMENT '"&amp; B80 &amp;"'," &amp; IF(A80="",""," */")</f>
+        <v>`name` VARCHAR(128) NOT NULL COMMENT '名前',</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B81" s="15" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="C81" s="15" t="s">
-        <v>40</v>
+        <v>59</v>
       </c>
       <c r="D81" s="15" t="s">
         <v>16</v>
       </c>
       <c r="E81" s="16"/>
-      <c r="F81" s="16"/>
+      <c r="F81" s="16" t="s">
+        <v>7</v>
+      </c>
       <c r="G81" s="16"/>
       <c r="H81" s="17"/>
       <c r="I81" s="36" t="str">
-        <f t="shared" ref="I81:I85" si="11">IF(A81="","","/* ") &amp; "`" &amp; C81 &amp; "` " &amp; D81 &amp; IF(E81&gt;0,"(" &amp; E81 &amp; ") "," ") &amp; IF(F81&lt;&gt;"","NOT NULL ","") &amp; IF(G81="","","DEFAULT '" &amp; G81 &amp; "' ") &amp; "COMMENT '"&amp; B81 &amp;"'," &amp; IF(A81="",""," */")</f>
-        <v>`position` INT COMMENT 'position',</v>
+        <f t="shared" si="8"/>
+        <v>`ord` INT NOT NULL COMMENT 'ord',</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A82" s="22"/>
       <c r="B82" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="C82" s="15" t="s">
-        <v>12</v>
+        <v>0</v>
+      </c>
+      <c r="C82" s="18" t="s">
+        <v>10</v>
       </c>
       <c r="D82" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="E82" s="16">
-        <v>128</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="E82" s="16"/>
       <c r="F82" s="16"/>
       <c r="G82" s="16"/>
       <c r="H82" s="17"/>
       <c r="I82" s="36" t="str">
-        <f t="shared" si="11"/>
-        <v>`name` VARCHAR(128) COMMENT '名前',</v>
+        <f t="shared" si="8"/>
+        <v>`created` DATETIME COMMENT '登録日',</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B83" s="15" t="s">
+      <c r="A83" s="22"/>
+      <c r="I83" s="37" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="D85" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="E85" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="F85" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="G85" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="H85" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="I85" s="30"/>
+    </row>
+    <row r="86" spans="1:9" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="B86" s="51" t="s">
+        <v>34</v>
+      </c>
+      <c r="C86" s="51" t="s">
+        <v>35</v>
+      </c>
+      <c r="D86" s="33"/>
+      <c r="E86" s="34"/>
+      <c r="F86" s="34"/>
+      <c r="G86" s="34"/>
+      <c r="H86" s="35"/>
+      <c r="I86" s="27" t="str">
+        <f xml:space="preserve"> "CREATE TABLE `" &amp; C86 &amp; "` ("</f>
+        <v>CREATE TABLE `todos` (</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="B87" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C87" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="D87" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E87" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F87" s="16"/>
+      <c r="G87" s="16"/>
+      <c r="H87" s="17"/>
+      <c r="I87" s="27" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="B88" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="C88" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="D88" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="E88" s="16"/>
+      <c r="F88" s="16"/>
+      <c r="G88" s="16"/>
+      <c r="H88" s="17"/>
+      <c r="I88" s="36" t="str">
+        <f t="shared" ref="I88" si="9">IF(A88="","","/* ") &amp; "`" &amp; C88 &amp; "` " &amp; D88 &amp; IF(E88&gt;0,"(" &amp; E88 &amp; ") "," ") &amp; IF(F88&lt;&gt;"","NOT NULL ","") &amp; IF(G88="","","DEFAULT '" &amp; G88 &amp; "' ") &amp; "COMMENT '"&amp; B88 &amp;"'," &amp; IF(A88="",""," */")</f>
+        <v>`todopage_id` INT COMMENT 'page',</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="B89" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C89" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="D89" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="E89" s="16"/>
+      <c r="F89" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="G89" s="16"/>
+      <c r="H89" s="17"/>
+      <c r="I89" s="36" t="str">
+        <f t="shared" ref="I89" si="10">IF(A89="","","/* ") &amp; "`" &amp; C89 &amp; "` " &amp; D89 &amp; IF(E89&gt;0,"(" &amp; E89 &amp; ") "," ") &amp; IF(F89&lt;&gt;"","NOT NULL ","") &amp; IF(G89="","","DEFAULT '" &amp; G89 &amp; "' ") &amp; "COMMENT '"&amp; B89 &amp;"'," &amp; IF(A89="",""," */")</f>
+        <v>`position` INT NOT NULL COMMENT 'position',</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="B90" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C90" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D90" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E90" s="16">
+        <v>128</v>
+      </c>
+      <c r="F90" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="G90" s="16"/>
+      <c r="H90" s="17"/>
+      <c r="I90" s="36" t="str">
+        <f t="shared" ref="I90:I93" si="11">IF(A90="","","/* ") &amp; "`" &amp; C90 &amp; "` " &amp; D90 &amp; IF(E90&gt;0,"(" &amp; E90 &amp; ") "," ") &amp; IF(F90&lt;&gt;"","NOT NULL ","") &amp; IF(G90="","","DEFAULT '" &amp; G90 &amp; "' ") &amp; "COMMENT '"&amp; B90 &amp;"'," &amp; IF(A90="",""," */")</f>
+        <v>`name` VARCHAR(128) NOT NULL COMMENT '名前',</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="B91" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="C83" s="15" t="s">
+      <c r="C91" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="D83" s="15" t="s">
+      <c r="D91" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="E83" s="16"/>
-      <c r="F83" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="G83" s="16">
+      <c r="E91" s="16"/>
+      <c r="F91" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="G91" s="16">
         <v>0</v>
       </c>
-      <c r="H83" s="17"/>
-      <c r="I83" s="36" t="str">
+      <c r="H91" s="17"/>
+      <c r="I91" s="36" t="str">
         <f t="shared" si="11"/>
         <v>`emphasis` BOOLEAN NOT NULL DEFAULT '0' COMMENT 'emphasis',</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A84" s="22"/>
-      <c r="B84" s="15" t="s">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A92" s="22"/>
+      <c r="B92" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C84" s="18" t="s">
+      <c r="C92" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="D84" s="15" t="s">
+      <c r="D92" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="E84" s="16"/>
-      <c r="F84" s="16"/>
-      <c r="G84" s="16"/>
-      <c r="H84" s="17"/>
-      <c r="I84" s="36" t="str">
-        <f t="shared" si="11"/>
-        <v>`created` DATETIME COMMENT '登録日',</v>
-      </c>
-    </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A85" s="22"/>
-      <c r="B85" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="C85" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="D85" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="E85" s="16"/>
-      <c r="F85" s="16"/>
-      <c r="G85" s="16"/>
-      <c r="H85" s="17"/>
-      <c r="I85" s="36" t="str">
-        <f t="shared" si="11"/>
-        <v>`completed` DATE COMMENT '完了日',</v>
-      </c>
-    </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A86" s="22"/>
-      <c r="I86" s="37" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B88" s="42" t="s">
-        <v>62</v>
-      </c>
-      <c r="D88" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="E88" s="31" t="s">
-        <v>5</v>
-      </c>
-      <c r="F88" s="31" t="s">
-        <v>7</v>
-      </c>
-      <c r="G88" s="31" t="s">
-        <v>8</v>
-      </c>
-      <c r="H88" s="32" t="s">
-        <v>18</v>
-      </c>
-      <c r="I88" s="30"/>
-    </row>
-    <row r="89" spans="1:9" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="B89" s="51" t="s">
-        <v>62</v>
-      </c>
-      <c r="C89" s="51" t="s">
-        <v>63</v>
-      </c>
-      <c r="D89" s="33"/>
-      <c r="E89" s="34"/>
-      <c r="F89" s="34"/>
-      <c r="G89" s="34"/>
-      <c r="H89" s="35"/>
-      <c r="I89" s="27" t="str">
-        <f xml:space="preserve"> "CREATE TABLE `" &amp; C89 &amp; "` ("</f>
-        <v>CREATE TABLE `events` (</v>
-      </c>
-    </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B90" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="C90" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="D90" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="E90" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="F90" s="16"/>
-      <c r="G90" s="16"/>
-      <c r="H90" s="17"/>
-      <c r="I90" s="27" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B91" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="C91" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="D91" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="E91" s="16"/>
-      <c r="F91" s="16"/>
-      <c r="G91" s="16"/>
-      <c r="H91" s="17"/>
-      <c r="I91" s="36" t="str">
-        <f t="shared" ref="I91" si="12">IF(A91="","","/* ") &amp; "`" &amp; C91 &amp; "` " &amp; D91 &amp; IF(E91&gt;0,"(" &amp; E91 &amp; ") "," ") &amp; IF(F91&lt;&gt;"","NOT NULL ","") &amp; IF(G91="","","DEFAULT '" &amp; G91 &amp; "' ") &amp; "COMMENT '"&amp; B91 &amp;"'," &amp; IF(A91="",""," */")</f>
-        <v>`calendar_id` INT COMMENT 'calendars',</v>
-      </c>
-    </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B92" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="C92" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="D92" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="E92" s="16">
-        <v>128</v>
-      </c>
-      <c r="F92" s="16" t="s">
-        <v>7</v>
-      </c>
+      <c r="E92" s="16"/>
+      <c r="F92" s="16"/>
       <c r="G92" s="16"/>
       <c r="H92" s="17"/>
       <c r="I92" s="36" t="str">
-        <f t="shared" ref="I92:I98" si="13">IF(A92="","","/* ") &amp; "`" &amp; C92 &amp; "` " &amp; D92 &amp; IF(E92&gt;0,"(" &amp; E92 &amp; ") "," ") &amp; IF(F92&lt;&gt;"","NOT NULL ","") &amp; IF(G92="","","DEFAULT '" &amp; G92 &amp; "' ") &amp; "COMMENT '"&amp; B92 &amp;"'," &amp; IF(A92="",""," */")</f>
-        <v>`title` VARCHAR(128) NOT NULL COMMENT '名前',</v>
+        <f t="shared" si="11"/>
+        <v>`created` DATETIME COMMENT '登録日',</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A93" s="22"/>
       <c r="B93" s="15" t="s">
-        <v>64</v>
+        <v>38</v>
       </c>
       <c r="C93" s="15" t="s">
-        <v>67</v>
+        <v>39</v>
       </c>
       <c r="D93" s="15" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="E93" s="16"/>
-      <c r="F93" s="16" t="s">
-        <v>7</v>
-      </c>
+      <c r="F93" s="16"/>
       <c r="G93" s="16"/>
       <c r="H93" s="17"/>
       <c r="I93" s="36" t="str">
-        <f t="shared" si="13"/>
-        <v>`start` DATE NOT NULL COMMENT 'dayofevent',</v>
+        <f t="shared" si="11"/>
+        <v>`completed` DATE COMMENT '完了日',</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B94" s="15" t="s">
-        <v>68</v>
-      </c>
-      <c r="C94" s="15" t="s">
-        <v>68</v>
-      </c>
-      <c r="D94" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="E94" s="16"/>
-      <c r="F94" s="16"/>
-      <c r="G94" s="16"/>
-      <c r="H94" s="17"/>
-      <c r="I94" s="36" t="str">
-        <f t="shared" ref="I94:I95" si="14">IF(A94="","","/* ") &amp; "`" &amp; C94 &amp; "` " &amp; D94 &amp; IF(E94&gt;0,"(" &amp; E94 &amp; ") "," ") &amp; IF(F94&lt;&gt;"","NOT NULL ","") &amp; IF(G94="","","DEFAULT '" &amp; G94 &amp; "' ") &amp; "COMMENT '"&amp; B94 &amp;"'," &amp; IF(A94="",""," */")</f>
-        <v>`end` DATE COMMENT 'end',</v>
-      </c>
-    </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B95" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="C95" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="D95" s="15" t="s">
-        <v>75</v>
-      </c>
-      <c r="E95" s="16"/>
-      <c r="F95" s="16"/>
-      <c r="G95" s="16"/>
-      <c r="H95" s="17"/>
-      <c r="I95" s="36" t="str">
-        <f t="shared" si="14"/>
-        <v>`detail` TEXT COMMENT 'detail',</v>
+      <c r="A94" s="22"/>
+      <c r="I94" s="37" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B96" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="C96" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="D96" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="E96" s="16">
-        <v>32</v>
-      </c>
-      <c r="F96" s="16"/>
-      <c r="G96" s="16"/>
-      <c r="H96" s="17"/>
-      <c r="I96" s="36" t="str">
-        <f t="shared" si="13"/>
-        <v>`color` VARCHAR(32) COMMENT 'color',</v>
-      </c>
-    </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B97" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="C97" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="D97" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="E97" s="16">
-        <v>32</v>
-      </c>
-      <c r="F97" s="16"/>
-      <c r="G97" s="16"/>
-      <c r="H97" s="17"/>
-      <c r="I97" s="36" t="str">
-        <f t="shared" ref="I97" si="15">IF(A97="","","/* ") &amp; "`" &amp; C97 &amp; "` " &amp; D97 &amp; IF(E97&gt;0,"(" &amp; E97 &amp; ") "," ") &amp; IF(F97&lt;&gt;"","NOT NULL ","") &amp; IF(G97="","","DEFAULT '" &amp; G97 &amp; "' ") &amp; "COMMENT '"&amp; B97 &amp;"'," &amp; IF(A97="",""," */")</f>
-        <v>`textcolor` VARCHAR(32) COMMENT 'textcolor',</v>
+      <c r="D96" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="E96" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="F96" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="G96" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="H96" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="I96" s="30"/>
+    </row>
+    <row r="97" spans="1:9" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="B97" s="51" t="s">
+        <v>41</v>
+      </c>
+      <c r="C97" s="51" t="s">
+        <v>42</v>
+      </c>
+      <c r="D97" s="33"/>
+      <c r="E97" s="34"/>
+      <c r="F97" s="34"/>
+      <c r="G97" s="34"/>
+      <c r="H97" s="35"/>
+      <c r="I97" s="27" t="str">
+        <f xml:space="preserve"> "CREATE TABLE `" &amp; C97 &amp; "` ("</f>
+        <v>CREATE TABLE `histories` (</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A98" s="22"/>
       <c r="B98" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="C98" s="18" t="s">
-        <v>10</v>
+        <v>9</v>
+      </c>
+      <c r="C98" s="15" t="s">
+        <v>1</v>
       </c>
       <c r="D98" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="E98" s="16"/>
+        <v>6</v>
+      </c>
+      <c r="E98" s="16" t="s">
+        <v>6</v>
+      </c>
       <c r="F98" s="16"/>
       <c r="G98" s="16"/>
       <c r="H98" s="17"/>
-      <c r="I98" s="36" t="str">
+      <c r="I98" s="27" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="B99" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="C99" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="D99" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="E99" s="16"/>
+      <c r="F99" s="16"/>
+      <c r="G99" s="16"/>
+      <c r="H99" s="17"/>
+      <c r="I99" s="36" t="str">
+        <f t="shared" ref="I99" si="12">IF(A99="","","/* ") &amp; "`" &amp; C99 &amp; "` " &amp; D99 &amp; IF(E99&gt;0,"(" &amp; E99 &amp; ") "," ") &amp; IF(F99&lt;&gt;"","NOT NULL ","") &amp; IF(G99="","","DEFAULT '" &amp; G99 &amp; "' ") &amp; "COMMENT '"&amp; B99 &amp;"'," &amp; IF(A99="",""," */")</f>
+        <v>`pageid` INT COMMENT 'page',</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="B100" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C100" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="D100" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="E100" s="16"/>
+      <c r="F100" s="16"/>
+      <c r="G100" s="16"/>
+      <c r="H100" s="17"/>
+      <c r="I100" s="36" t="str">
+        <f t="shared" ref="I100:I104" si="13">IF(A100="","","/* ") &amp; "`" &amp; C100 &amp; "` " &amp; D100 &amp; IF(E100&gt;0,"(" &amp; E100 &amp; ") "," ") &amp; IF(F100&lt;&gt;"","NOT NULL ","") &amp; IF(G100="","","DEFAULT '" &amp; G100 &amp; "' ") &amp; "COMMENT '"&amp; B100 &amp;"'," &amp; IF(A100="",""," */")</f>
+        <v>`position` INT COMMENT 'position',</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="B101" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C101" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D101" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E101" s="16">
+        <v>128</v>
+      </c>
+      <c r="F101" s="16"/>
+      <c r="G101" s="16"/>
+      <c r="H101" s="17"/>
+      <c r="I101" s="36" t="str">
         <f t="shared" si="13"/>
-        <v>`created` DATETIME COMMENT '登録日',</v>
-      </c>
-    </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A99" s="22"/>
-      <c r="I99" s="37" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B101" s="42"/>
-      <c r="D101" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="E101" s="31" t="s">
-        <v>5</v>
-      </c>
-      <c r="F101" s="31" t="s">
-        <v>7</v>
-      </c>
-      <c r="G101" s="31" t="s">
-        <v>8</v>
-      </c>
-      <c r="H101" s="32" t="s">
-        <v>18</v>
-      </c>
-      <c r="I101" s="30"/>
-    </row>
-    <row r="102" spans="1:9" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="B102" s="51" t="s">
-        <v>71</v>
-      </c>
-      <c r="C102" s="51" t="s">
-        <v>72</v>
-      </c>
-      <c r="D102" s="33"/>
-      <c r="E102" s="34"/>
-      <c r="F102" s="34"/>
-      <c r="G102" s="34"/>
-      <c r="H102" s="35"/>
-      <c r="I102" s="27" t="str">
-        <f xml:space="preserve"> "CREATE TABLE `" &amp; C102 &amp; "` ("</f>
-        <v>CREATE TABLE `calendars` (</v>
+        <v>`name` VARCHAR(128) COMMENT '名前',</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="B102" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="C102" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="D102" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="E102" s="16"/>
+      <c r="F102" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="G102" s="16">
+        <v>0</v>
+      </c>
+      <c r="H102" s="17"/>
+      <c r="I102" s="36" t="str">
+        <f t="shared" si="13"/>
+        <v>`emphasis` BOOLEAN NOT NULL DEFAULT '0' COMMENT 'emphasis',</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A103" s="22"/>
       <c r="B103" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="C103" s="15" t="s">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="C103" s="18" t="s">
+        <v>10</v>
       </c>
       <c r="D103" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="E103" s="16" t="s">
-        <v>6</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="E103" s="16"/>
       <c r="F103" s="16"/>
       <c r="G103" s="16"/>
       <c r="H103" s="17"/>
-      <c r="I103" s="27" t="s">
-        <v>3</v>
+      <c r="I103" s="36" t="str">
+        <f t="shared" si="13"/>
+        <v>`created` DATETIME COMMENT '登録日',</v>
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A104" s="22"/>
       <c r="B104" s="15" t="s">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="C104" s="15" t="s">
-        <v>12</v>
+        <v>39</v>
       </c>
       <c r="D104" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="E104" s="16">
-        <v>128</v>
-      </c>
-      <c r="F104" s="16" t="s">
-        <v>7</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="E104" s="16"/>
+      <c r="F104" s="16"/>
       <c r="G104" s="16"/>
       <c r="H104" s="17"/>
       <c r="I104" s="36" t="str">
-        <f t="shared" ref="I104:I106" si="16">IF(A104="","","/* ") &amp; "`" &amp; C104 &amp; "` " &amp; D104 &amp; IF(E104&gt;0,"(" &amp; E104 &amp; ") "," ") &amp; IF(F104&lt;&gt;"","NOT NULL ","") &amp; IF(G104="","","DEFAULT '" &amp; G104 &amp; "' ") &amp; "COMMENT '"&amp; B104 &amp;"'," &amp; IF(A104="",""," */")</f>
-        <v>`name` VARCHAR(128) NOT NULL COMMENT '名前',</v>
+        <f t="shared" si="13"/>
+        <v>`completed` DATE COMMENT '完了日',</v>
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B105" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="C105" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="D105" s="15" t="s">
+      <c r="A105" s="22"/>
+      <c r="I105" s="37" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="B107" s="42" t="s">
+        <v>62</v>
+      </c>
+      <c r="D107" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="E107" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="F107" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="G107" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="H107" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="I107" s="30"/>
+    </row>
+    <row r="108" spans="1:9" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="B108" s="51" t="s">
+        <v>62</v>
+      </c>
+      <c r="C108" s="51" t="s">
+        <v>63</v>
+      </c>
+      <c r="D108" s="33"/>
+      <c r="E108" s="34"/>
+      <c r="F108" s="34"/>
+      <c r="G108" s="34"/>
+      <c r="H108" s="35"/>
+      <c r="I108" s="27" t="str">
+        <f xml:space="preserve"> "CREATE TABLE `" &amp; C108 &amp; "` ("</f>
+        <v>CREATE TABLE `events` (</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="B109" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C109" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="D109" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E109" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F109" s="16"/>
+      <c r="G109" s="16"/>
+      <c r="H109" s="17"/>
+      <c r="I109" s="27" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="B110" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="C110" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="D110" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="E105" s="16"/>
-      <c r="F105" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="G105" s="16"/>
-      <c r="H105" s="17"/>
-      <c r="I105" s="36" t="str">
-        <f t="shared" si="16"/>
-        <v>`position` INT NOT NULL COMMENT 'position',</v>
-      </c>
-    </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A106" s="22"/>
-      <c r="B106" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="C106" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="D106" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="E106" s="16"/>
-      <c r="F106" s="16"/>
-      <c r="G106" s="16"/>
-      <c r="H106" s="17"/>
-      <c r="I106" s="36" t="str">
-        <f t="shared" si="16"/>
-        <v>`created` DATETIME COMMENT '登録日',</v>
-      </c>
-    </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A107" s="22"/>
-      <c r="I107" s="37" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B109" s="42" t="s">
-        <v>61</v>
-      </c>
-      <c r="D109" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="E109" s="31" t="s">
-        <v>5</v>
-      </c>
-      <c r="F109" s="31" t="s">
-        <v>7</v>
-      </c>
-      <c r="G109" s="31" t="s">
-        <v>8</v>
-      </c>
-      <c r="H109" s="32" t="s">
-        <v>18</v>
-      </c>
-      <c r="I109" s="30"/>
-    </row>
-    <row r="110" spans="1:9" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="B110" s="51" t="s">
-        <v>52</v>
-      </c>
-      <c r="C110" s="51" t="s">
-        <v>30</v>
-      </c>
-      <c r="D110" s="33"/>
-      <c r="E110" s="34"/>
-      <c r="F110" s="34"/>
-      <c r="G110" s="34"/>
-      <c r="H110" s="35"/>
-      <c r="I110" s="27" t="str">
-        <f xml:space="preserve"> "CREATE TABLE `" &amp; C110 &amp; "` ("</f>
-        <v>CREATE TABLE `categories` (</v>
+      <c r="E110" s="16"/>
+      <c r="F110" s="16"/>
+      <c r="G110" s="16"/>
+      <c r="H110" s="17"/>
+      <c r="I110" s="36" t="str">
+        <f t="shared" ref="I110" si="14">IF(A110="","","/* ") &amp; "`" &amp; C110 &amp; "` " &amp; D110 &amp; IF(E110&gt;0,"(" &amp; E110 &amp; ") "," ") &amp; IF(F110&lt;&gt;"","NOT NULL ","") &amp; IF(G110="","","DEFAULT '" &amp; G110 &amp; "' ") &amp; "COMMENT '"&amp; B110 &amp;"'," &amp; IF(A110="",""," */")</f>
+        <v>`calendar_id` INT COMMENT 'calendars',</v>
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B111" s="15" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C111" s="15" t="s">
-        <v>1</v>
+        <v>66</v>
       </c>
       <c r="D111" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="E111" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="F111" s="16"/>
+        <v>13</v>
+      </c>
+      <c r="E111" s="16">
+        <v>128</v>
+      </c>
+      <c r="F111" s="16" t="s">
+        <v>7</v>
+      </c>
       <c r="G111" s="16"/>
       <c r="H111" s="17"/>
-      <c r="I111" s="27" t="s">
-        <v>3</v>
+      <c r="I111" s="36" t="str">
+        <f t="shared" ref="I111:I117" si="15">IF(A111="","","/* ") &amp; "`" &amp; C111 &amp; "` " &amp; D111 &amp; IF(E111&gt;0,"(" &amp; E111 &amp; ") "," ") &amp; IF(F111&lt;&gt;"","NOT NULL ","") &amp; IF(G111="","","DEFAULT '" &amp; G111 &amp; "' ") &amp; "COMMENT '"&amp; B111 &amp;"'," &amp; IF(A111="",""," */")</f>
+        <v>`title` VARCHAR(128) NOT NULL COMMENT '名前',</v>
       </c>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B112" s="15" t="s">
-        <v>15</v>
+        <v>64</v>
       </c>
       <c r="C112" s="15" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="D112" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="E112" s="16">
-        <v>128</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="E112" s="16"/>
       <c r="F112" s="16" t="s">
         <v>7</v>
       </c>
       <c r="G112" s="16"/>
       <c r="H112" s="17"/>
       <c r="I112" s="36" t="str">
-        <f t="shared" ref="I112" si="17">IF(A112="","","/* ") &amp; "`" &amp; C112 &amp; "` " &amp; D112 &amp; IF(E112&gt;0,"(" &amp; E112 &amp; ") "," ") &amp; IF(F112&lt;&gt;"","NOT NULL ","") &amp; IF(G112="","","DEFAULT '" &amp; G112 &amp; "' ") &amp; "COMMENT '"&amp; B112 &amp;"'," &amp; IF(A112="",""," */")</f>
-        <v>`name` VARCHAR(128) NOT NULL COMMENT '名前',</v>
+        <f t="shared" si="15"/>
+        <v>`start` DATE NOT NULL COMMENT 'dayofevent',</v>
       </c>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B113" s="15" t="s">
-        <v>36</v>
+        <v>68</v>
       </c>
       <c r="C113" s="15" t="s">
-        <v>36</v>
+        <v>68</v>
       </c>
       <c r="D113" s="15" t="s">
-        <v>16</v>
+        <v>65</v>
       </c>
       <c r="E113" s="16"/>
-      <c r="F113" s="16" t="s">
-        <v>7</v>
-      </c>
+      <c r="F113" s="16"/>
       <c r="G113" s="16"/>
       <c r="H113" s="17"/>
       <c r="I113" s="36" t="str">
-        <f t="shared" ref="I113" si="18">IF(A113="","","/* ") &amp; "`" &amp; C113 &amp; "` " &amp; D113 &amp; IF(E113&gt;0,"(" &amp; E113 &amp; ") "," ") &amp; IF(F113&lt;&gt;"","NOT NULL ","") &amp; IF(G113="","","DEFAULT '" &amp; G113 &amp; "' ") &amp; "COMMENT '"&amp; B113 &amp;"'," &amp; IF(A113="",""," */")</f>
-        <v>`position` INT NOT NULL COMMENT 'position',</v>
+        <f t="shared" ref="I113:I114" si="16">IF(A113="","","/* ") &amp; "`" &amp; C113 &amp; "` " &amp; D113 &amp; IF(E113&gt;0,"(" &amp; E113 &amp; ") "," ") &amp; IF(F113&lt;&gt;"","NOT NULL ","") &amp; IF(G113="","","DEFAULT '" &amp; G113 &amp; "' ") &amp; "COMMENT '"&amp; B113 &amp;"'," &amp; IF(A113="",""," */")</f>
+        <v>`end` DATE COMMENT 'end',</v>
       </c>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A114" s="22"/>
-      <c r="I114" s="37" t="s">
+      <c r="B114" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="C114" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="D114" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="E114" s="16"/>
+      <c r="F114" s="16"/>
+      <c r="G114" s="16"/>
+      <c r="H114" s="17"/>
+      <c r="I114" s="36" t="str">
+        <f t="shared" si="16"/>
+        <v>`detail` TEXT COMMENT 'detail',</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="B115" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="C115" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="D115" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E115" s="16">
+        <v>32</v>
+      </c>
+      <c r="F115" s="16"/>
+      <c r="G115" s="16"/>
+      <c r="H115" s="17"/>
+      <c r="I115" s="36" t="str">
+        <f t="shared" si="15"/>
+        <v>`color` VARCHAR(32) COMMENT 'color',</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="B116" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="C116" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="D116" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E116" s="16">
+        <v>32</v>
+      </c>
+      <c r="F116" s="16"/>
+      <c r="G116" s="16"/>
+      <c r="H116" s="17"/>
+      <c r="I116" s="36" t="str">
+        <f t="shared" ref="I116" si="17">IF(A116="","","/* ") &amp; "`" &amp; C116 &amp; "` " &amp; D116 &amp; IF(E116&gt;0,"(" &amp; E116 &amp; ") "," ") &amp; IF(F116&lt;&gt;"","NOT NULL ","") &amp; IF(G116="","","DEFAULT '" &amp; G116 &amp; "' ") &amp; "COMMENT '"&amp; B116 &amp;"'," &amp; IF(A116="",""," */")</f>
+        <v>`textcolor` VARCHAR(32) COMMENT 'textcolor',</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A117" s="22"/>
+      <c r="B117" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C117" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="D117" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E117" s="16"/>
+      <c r="F117" s="16"/>
+      <c r="G117" s="16"/>
+      <c r="H117" s="17"/>
+      <c r="I117" s="36" t="str">
+        <f t="shared" si="15"/>
+        <v>`created` DATETIME COMMENT '登録日',</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A118" s="22"/>
+      <c r="I118" s="37" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="D116" s="30" t="s">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="B120" s="42"/>
+      <c r="D120" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="E116" s="31" t="s">
+      <c r="E120" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="F116" s="31" t="s">
+      <c r="F120" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="G116" s="31" t="s">
+      <c r="G120" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="H116" s="32" t="s">
+      <c r="H120" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="I116" s="30"/>
-    </row>
-    <row r="117" spans="1:9" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="B117" s="51" t="s">
-        <v>43</v>
-      </c>
-      <c r="C117" s="51" t="s">
-        <v>44</v>
-      </c>
-      <c r="D117" s="33"/>
-      <c r="E117" s="34"/>
-      <c r="F117" s="34"/>
-      <c r="G117" s="34"/>
-      <c r="H117" s="35"/>
-      <c r="I117" s="27" t="str">
-        <f xml:space="preserve"> "CREATE TABLE `" &amp; C117 &amp; "` ("</f>
-        <v>CREATE TABLE `notes` (</v>
-      </c>
-    </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B118" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="C118" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="D118" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="E118" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="F118" s="16"/>
-      <c r="G118" s="16"/>
-      <c r="H118" s="17"/>
-      <c r="I118" s="27" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B119" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="C119" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="D119" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="E119" s="16"/>
-      <c r="F119" s="16"/>
-      <c r="G119" s="16"/>
-      <c r="H119" s="17"/>
-      <c r="I119" s="36" t="str">
-        <f t="shared" ref="I119" si="19">IF(A119="","","/* ") &amp; "`" &amp; C119 &amp; "` " &amp; D119 &amp; IF(E119&gt;0,"(" &amp; E119 &amp; ") "," ") &amp; IF(F119&lt;&gt;"","NOT NULL ","") &amp; IF(G119="","","DEFAULT '" &amp; G119 &amp; "' ") &amp; "COMMENT '"&amp; B119 &amp;"'," &amp; IF(A119="",""," */")</f>
-        <v>`category_id` INT COMMENT '分類',</v>
-      </c>
-    </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B120" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="C120" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="D120" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="E120" s="16">
-        <v>64</v>
-      </c>
-      <c r="F120" s="16"/>
-      <c r="G120" s="16"/>
-      <c r="H120" s="17"/>
-      <c r="I120" s="36" t="str">
-        <f t="shared" ref="I120:I125" si="20">IF(A120="","","/* ") &amp; "`" &amp; C120 &amp; "` " &amp; D120 &amp; IF(E120&gt;0,"(" &amp; E120 &amp; ") "," ") &amp; IF(F120&lt;&gt;"","NOT NULL ","") &amp; IF(G120="","","DEFAULT '" &amp; G120 &amp; "' ") &amp; "COMMENT '"&amp; B120 &amp;"'," &amp; IF(A120="",""," */")</f>
-        <v>`name` VARCHAR(64) COMMENT '名前',</v>
-      </c>
-    </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B121" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="C121" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="D121" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="E121" s="16"/>
-      <c r="F121" s="16"/>
-      <c r="G121" s="16"/>
-      <c r="H121" s="17"/>
-      <c r="I121" s="36" t="str">
-        <f t="shared" si="20"/>
-        <v>`text` TEXT COMMENT 'テキスト',</v>
+      <c r="I120" s="30"/>
+    </row>
+    <row r="121" spans="1:9" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="B121" s="51" t="s">
+        <v>71</v>
+      </c>
+      <c r="C121" s="51" t="s">
+        <v>72</v>
+      </c>
+      <c r="D121" s="33"/>
+      <c r="E121" s="34"/>
+      <c r="F121" s="34"/>
+      <c r="G121" s="34"/>
+      <c r="H121" s="35"/>
+      <c r="I121" s="27" t="str">
+        <f xml:space="preserve"> "CREATE TABLE `" &amp; C121 &amp; "` ("</f>
+        <v>CREATE TABLE `calendars` (</v>
       </c>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B122" s="15" t="s">
-        <v>48</v>
+        <v>9</v>
       </c>
       <c r="C122" s="15" t="s">
-        <v>49</v>
+        <v>1</v>
       </c>
       <c r="D122" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="E122" s="16">
-        <v>32</v>
+        <v>6</v>
+      </c>
+      <c r="E122" s="16" t="s">
+        <v>6</v>
       </c>
       <c r="F122" s="16"/>
       <c r="G122" s="16"/>
       <c r="H122" s="17"/>
-      <c r="I122" s="36" t="str">
-        <f t="shared" si="20"/>
-        <v>`xyz` VARCHAR(32) COMMENT 'xyz',</v>
+      <c r="I122" s="27" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B123" s="15" t="s">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="C123" s="15" t="s">
-        <v>51</v>
+        <v>12</v>
       </c>
       <c r="D123" s="15" t="s">
         <v>13</v>
       </c>
       <c r="E123" s="16">
-        <v>32</v>
-      </c>
-      <c r="F123" s="16"/>
+        <v>128</v>
+      </c>
+      <c r="F123" s="16" t="s">
+        <v>7</v>
+      </c>
       <c r="G123" s="16"/>
       <c r="H123" s="17"/>
       <c r="I123" s="36" t="str">
-        <f t="shared" ref="I123" si="21">IF(A123="","","/* ") &amp; "`" &amp; C123 &amp; "` " &amp; D123 &amp; IF(E123&gt;0,"(" &amp; E123 &amp; ") "," ") &amp; IF(F123&lt;&gt;"","NOT NULL ","") &amp; IF(G123="","","DEFAULT '" &amp; G123 &amp; "' ") &amp; "COMMENT '"&amp; B123 &amp;"'," &amp; IF(A123="",""," */")</f>
-        <v>`wh` VARCHAR(32) COMMENT 'wh',</v>
+        <f t="shared" ref="I123:I125" si="18">IF(A123="","","/* ") &amp; "`" &amp; C123 &amp; "` " &amp; D123 &amp; IF(E123&gt;0,"(" &amp; E123 &amp; ") "," ") &amp; IF(F123&lt;&gt;"","NOT NULL ","") &amp; IF(G123="","","DEFAULT '" &amp; G123 &amp; "' ") &amp; "COMMENT '"&amp; B123 &amp;"'," &amp; IF(A123="",""," */")</f>
+        <v>`name` VARCHAR(128) NOT NULL COMMENT '名前',</v>
       </c>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B124" s="15" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="C124" s="15" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="D124" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="E124" s="16">
-        <v>32</v>
-      </c>
-      <c r="F124" s="16"/>
+        <v>16</v>
+      </c>
+      <c r="E124" s="16"/>
+      <c r="F124" s="16" t="s">
+        <v>7</v>
+      </c>
       <c r="G124" s="16"/>
       <c r="H124" s="17"/>
       <c r="I124" s="36" t="str">
-        <f t="shared" si="20"/>
-        <v>`color` VARCHAR(32) COMMENT 'color',</v>
+        <f t="shared" si="18"/>
+        <v>`position` INT NOT NULL COMMENT 'position',</v>
       </c>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.15">
@@ -4017,7 +4220,7 @@
       <c r="G125" s="16"/>
       <c r="H125" s="17"/>
       <c r="I125" s="36" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>`created` DATETIME COMMENT '登録日',</v>
       </c>
     </row>
@@ -4027,330 +4230,701 @@
         <v>2</v>
       </c>
     </row>
+    <row r="128" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="B128" s="42" t="s">
+        <v>61</v>
+      </c>
+      <c r="D128" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="E128" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="F128" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="G128" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="H128" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="I128" s="30"/>
+    </row>
+    <row r="129" spans="1:9" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="B129" s="51" t="s">
+        <v>52</v>
+      </c>
+      <c r="C129" s="51" t="s">
+        <v>30</v>
+      </c>
+      <c r="D129" s="33"/>
+      <c r="E129" s="34"/>
+      <c r="F129" s="34"/>
+      <c r="G129" s="34"/>
+      <c r="H129" s="35"/>
+      <c r="I129" s="27" t="str">
+        <f xml:space="preserve"> "CREATE TABLE `" &amp; C129 &amp; "` ("</f>
+        <v>CREATE TABLE `categories` (</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="B130" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C130" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="D130" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E130" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F130" s="16"/>
+      <c r="G130" s="16"/>
+      <c r="H130" s="17"/>
+      <c r="I130" s="27" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="131" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="B131" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C131" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D131" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E131" s="16">
+        <v>128</v>
+      </c>
+      <c r="F131" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="G131" s="16"/>
+      <c r="H131" s="17"/>
+      <c r="I131" s="36" t="str">
+        <f t="shared" ref="I131" si="19">IF(A131="","","/* ") &amp; "`" &amp; C131 &amp; "` " &amp; D131 &amp; IF(E131&gt;0,"(" &amp; E131 &amp; ") "," ") &amp; IF(F131&lt;&gt;"","NOT NULL ","") &amp; IF(G131="","","DEFAULT '" &amp; G131 &amp; "' ") &amp; "COMMENT '"&amp; B131 &amp;"'," &amp; IF(A131="",""," */")</f>
+        <v>`name` VARCHAR(128) NOT NULL COMMENT '名前',</v>
+      </c>
+    </row>
+    <row r="132" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="B132" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C132" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="D132" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="E132" s="16"/>
+      <c r="F132" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="G132" s="16"/>
+      <c r="H132" s="17"/>
+      <c r="I132" s="36" t="str">
+        <f t="shared" ref="I132" si="20">IF(A132="","","/* ") &amp; "`" &amp; C132 &amp; "` " &amp; D132 &amp; IF(E132&gt;0,"(" &amp; E132 &amp; ") "," ") &amp; IF(F132&lt;&gt;"","NOT NULL ","") &amp; IF(G132="","","DEFAULT '" &amp; G132 &amp; "' ") &amp; "COMMENT '"&amp; B132 &amp;"'," &amp; IF(A132="",""," */")</f>
+        <v>`position` INT NOT NULL COMMENT 'position',</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A133" s="22"/>
+      <c r="I133" s="37" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="135" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="D135" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="E135" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="F135" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="G135" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="H135" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="I135" s="30"/>
+    </row>
+    <row r="136" spans="1:9" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="B136" s="51" t="s">
+        <v>43</v>
+      </c>
+      <c r="C136" s="51" t="s">
+        <v>44</v>
+      </c>
+      <c r="D136" s="33"/>
+      <c r="E136" s="34"/>
+      <c r="F136" s="34"/>
+      <c r="G136" s="34"/>
+      <c r="H136" s="35"/>
+      <c r="I136" s="27" t="str">
+        <f xml:space="preserve"> "CREATE TABLE `" &amp; C136 &amp; "` ("</f>
+        <v>CREATE TABLE `notes` (</v>
+      </c>
+    </row>
+    <row r="137" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="B137" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C137" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="D137" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E137" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F137" s="16"/>
+      <c r="G137" s="16"/>
+      <c r="H137" s="17"/>
+      <c r="I137" s="27" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="138" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="B138" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="C138" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="D138" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="E138" s="16"/>
+      <c r="F138" s="16"/>
+      <c r="G138" s="16"/>
+      <c r="H138" s="17"/>
+      <c r="I138" s="36" t="str">
+        <f t="shared" ref="I138" si="21">IF(A138="","","/* ") &amp; "`" &amp; C138 &amp; "` " &amp; D138 &amp; IF(E138&gt;0,"(" &amp; E138 &amp; ") "," ") &amp; IF(F138&lt;&gt;"","NOT NULL ","") &amp; IF(G138="","","DEFAULT '" &amp; G138 &amp; "' ") &amp; "COMMENT '"&amp; B138 &amp;"'," &amp; IF(A138="",""," */")</f>
+        <v>`category_id` INT COMMENT '分類',</v>
+      </c>
+    </row>
+    <row r="139" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="B139" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C139" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D139" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E139" s="16">
+        <v>64</v>
+      </c>
+      <c r="F139" s="16"/>
+      <c r="G139" s="16"/>
+      <c r="H139" s="17"/>
+      <c r="I139" s="36" t="str">
+        <f t="shared" ref="I139:I144" si="22">IF(A139="","","/* ") &amp; "`" &amp; C139 &amp; "` " &amp; D139 &amp; IF(E139&gt;0,"(" &amp; E139 &amp; ") "," ") &amp; IF(F139&lt;&gt;"","NOT NULL ","") &amp; IF(G139="","","DEFAULT '" &amp; G139 &amp; "' ") &amp; "COMMENT '"&amp; B139 &amp;"'," &amp; IF(A139="",""," */")</f>
+        <v>`name` VARCHAR(64) COMMENT '名前',</v>
+      </c>
+    </row>
+    <row r="140" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="B140" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="C140" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="D140" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E140" s="16"/>
+      <c r="F140" s="16"/>
+      <c r="G140" s="16"/>
+      <c r="H140" s="17"/>
+      <c r="I140" s="36" t="str">
+        <f t="shared" si="22"/>
+        <v>`text` TEXT COMMENT 'テキスト',</v>
+      </c>
+    </row>
+    <row r="141" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="B141" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="C141" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="D141" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E141" s="16">
+        <v>32</v>
+      </c>
+      <c r="F141" s="16"/>
+      <c r="G141" s="16"/>
+      <c r="H141" s="17"/>
+      <c r="I141" s="36" t="str">
+        <f t="shared" si="22"/>
+        <v>`xyz` VARCHAR(32) COMMENT 'xyz',</v>
+      </c>
+    </row>
+    <row r="142" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="B142" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C142" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="D142" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E142" s="16">
+        <v>32</v>
+      </c>
+      <c r="F142" s="16"/>
+      <c r="G142" s="16"/>
+      <c r="H142" s="17"/>
+      <c r="I142" s="36" t="str">
+        <f t="shared" ref="I142" si="23">IF(A142="","","/* ") &amp; "`" &amp; C142 &amp; "` " &amp; D142 &amp; IF(E142&gt;0,"(" &amp; E142 &amp; ") "," ") &amp; IF(F142&lt;&gt;"","NOT NULL ","") &amp; IF(G142="","","DEFAULT '" &amp; G142 &amp; "' ") &amp; "COMMENT '"&amp; B142 &amp;"'," &amp; IF(A142="",""," */")</f>
+        <v>`wh` VARCHAR(32) COMMENT 'wh',</v>
+      </c>
+    </row>
+    <row r="143" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="B143" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="C143" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="D143" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E143" s="16">
+        <v>32</v>
+      </c>
+      <c r="F143" s="16"/>
+      <c r="G143" s="16"/>
+      <c r="H143" s="17"/>
+      <c r="I143" s="36" t="str">
+        <f t="shared" si="22"/>
+        <v>`color` VARCHAR(32) COMMENT 'color',</v>
+      </c>
+    </row>
+    <row r="144" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A144" s="22"/>
+      <c r="B144" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C144" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="D144" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E144" s="16"/>
+      <c r="F144" s="16"/>
+      <c r="G144" s="16"/>
+      <c r="H144" s="17"/>
+      <c r="I144" s="36" t="str">
+        <f t="shared" si="22"/>
+        <v>`created` DATETIME COMMENT '登録日',</v>
+      </c>
+    </row>
+    <row r="145" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A145" s="22"/>
+      <c r="I145" s="37" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="7"/>
-  <conditionalFormatting sqref="B1:B3 B73:B75 B125:B126 B114 B15 B22 B11 B33 B41 B52:B57 B128:B1048576">
-    <cfRule type="expression" dxfId="64" priority="162">
+  <conditionalFormatting sqref="B1:B3 B92:B94 B144:B145 B133 B15 B22 B11 B33 B60 B71:B76 B147:B1048576">
+    <cfRule type="expression" dxfId="88" priority="174">
       <formula>A1&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B66:B68 B71:B72">
-    <cfRule type="expression" dxfId="63" priority="106">
-      <formula>A66&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B76">
-    <cfRule type="expression" dxfId="62" priority="96">
-      <formula>A76&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B70">
-    <cfRule type="expression" dxfId="61" priority="76">
-      <formula>A70&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B84:B86">
-    <cfRule type="expression" dxfId="60" priority="74">
+  <conditionalFormatting sqref="B85:B87 B90:B91">
+    <cfRule type="expression" dxfId="87" priority="118">
+      <formula>A85&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B95">
+    <cfRule type="expression" dxfId="86" priority="108">
+      <formula>A95&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B89">
+    <cfRule type="expression" dxfId="85" priority="88">
+      <formula>A89&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B103:B105">
+    <cfRule type="expression" dxfId="84" priority="86">
+      <formula>A103&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B96:B98 B101">
+    <cfRule type="expression" dxfId="83" priority="85">
+      <formula>A96&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B106">
+    <cfRule type="expression" dxfId="82" priority="84">
+      <formula>A106&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B100">
+    <cfRule type="expression" dxfId="81" priority="83">
+      <formula>A100&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B135:B137 B143 B139:B141">
+    <cfRule type="expression" dxfId="80" priority="81">
+      <formula>A135&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B146">
+    <cfRule type="expression" dxfId="79" priority="80">
+      <formula>A146&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B142">
+    <cfRule type="expression" dxfId="78" priority="78">
+      <formula>A142&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B128:B131">
+    <cfRule type="expression" dxfId="77" priority="76">
+      <formula>A128&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B134">
+    <cfRule type="expression" dxfId="76" priority="75">
+      <formula>A134&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B138">
+    <cfRule type="expression" dxfId="75" priority="73">
+      <formula>A138&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B132">
+    <cfRule type="expression" dxfId="74" priority="72">
+      <formula>A132&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B83">
+    <cfRule type="expression" dxfId="73" priority="71">
+      <formula>A83&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B77:B80">
+    <cfRule type="expression" dxfId="72" priority="70">
+      <formula>A77&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B84">
+    <cfRule type="expression" dxfId="71" priority="69">
       <formula>A84&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B77:B79 B82">
-    <cfRule type="expression" dxfId="59" priority="73">
-      <formula>A77&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B87">
-    <cfRule type="expression" dxfId="58" priority="72">
-      <formula>A87&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="B81">
-    <cfRule type="expression" dxfId="57" priority="71">
+    <cfRule type="expression" dxfId="70" priority="68">
       <formula>A81&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B116:B118 B124 B120:B122">
-    <cfRule type="expression" dxfId="56" priority="69">
+  <conditionalFormatting sqref="B82">
+    <cfRule type="expression" dxfId="69" priority="67">
+      <formula>A82&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B88">
+    <cfRule type="expression" dxfId="68" priority="66">
+      <formula>A88&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B99">
+    <cfRule type="expression" dxfId="67" priority="65">
+      <formula>A99&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B118">
+    <cfRule type="expression" dxfId="66" priority="64">
+      <formula>A118&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B107:B109 B111">
+    <cfRule type="expression" dxfId="65" priority="63">
+      <formula>A107&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B119">
+    <cfRule type="expression" dxfId="64" priority="62">
+      <formula>A119&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B112">
+    <cfRule type="expression" dxfId="63" priority="61">
+      <formula>A112&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B117">
+    <cfRule type="expression" dxfId="62" priority="60">
+      <formula>A117&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B115">
+    <cfRule type="expression" dxfId="61" priority="59">
+      <formula>A115&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B113">
+    <cfRule type="expression" dxfId="60" priority="57">
+      <formula>A113&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B116">
+    <cfRule type="expression" dxfId="59" priority="56">
       <formula>A116&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="B126">
+    <cfRule type="expression" dxfId="58" priority="55">
+      <formula>A126&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B120:B123">
+    <cfRule type="expression" dxfId="57" priority="54">
+      <formula>A120&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="B127">
-    <cfRule type="expression" dxfId="55" priority="68">
+    <cfRule type="expression" dxfId="56" priority="53">
       <formula>A127&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B123">
-    <cfRule type="expression" dxfId="54" priority="66">
-      <formula>A123&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B109:B112">
-    <cfRule type="expression" dxfId="53" priority="64">
-      <formula>A109&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B115">
-    <cfRule type="expression" dxfId="52" priority="63">
-      <formula>A115&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B119">
-    <cfRule type="expression" dxfId="51" priority="61">
-      <formula>A119&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B113">
-    <cfRule type="expression" dxfId="50" priority="60">
-      <formula>A113&lt;&gt;""</formula>
+  <conditionalFormatting sqref="B124">
+    <cfRule type="expression" dxfId="55" priority="52">
+      <formula>A124&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B125">
+    <cfRule type="expression" dxfId="54" priority="51">
+      <formula>A125&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B110">
+    <cfRule type="expression" dxfId="53" priority="50">
+      <formula>A110&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B114">
+    <cfRule type="expression" dxfId="52" priority="49">
+      <formula>A114&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B102">
+    <cfRule type="expression" dxfId="51" priority="46">
+      <formula>A102&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B19:B21">
+    <cfRule type="expression" dxfId="50" priority="45">
+      <formula>A19&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B12:B14">
+    <cfRule type="expression" dxfId="49" priority="44">
+      <formula>A12&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B17">
+    <cfRule type="expression" dxfId="48" priority="43">
+      <formula>A17&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B10">
+    <cfRule type="expression" dxfId="47" priority="41">
+      <formula>A10&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B4:B7">
+    <cfRule type="expression" dxfId="46" priority="40">
+      <formula>A4&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B9">
+    <cfRule type="expression" dxfId="45" priority="38">
+      <formula>A9&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B16">
+    <cfRule type="expression" dxfId="44" priority="37">
+      <formula>A16&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B8">
+    <cfRule type="expression" dxfId="43" priority="36">
+      <formula>A8&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B23:B24">
+    <cfRule type="expression" dxfId="42" priority="33">
+      <formula>A23&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B18">
+    <cfRule type="expression" dxfId="41" priority="30">
+      <formula>A18&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B26">
+    <cfRule type="expression" dxfId="40" priority="29">
+      <formula>A26&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B30:B32">
+    <cfRule type="expression" dxfId="39" priority="28">
+      <formula>A30&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B25">
+    <cfRule type="expression" dxfId="38" priority="27">
+      <formula>A25&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B28">
+    <cfRule type="expression" dxfId="37" priority="26">
+      <formula>A28&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B27">
+    <cfRule type="expression" dxfId="36" priority="25">
+      <formula>A27&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B29">
+    <cfRule type="expression" dxfId="35" priority="24">
+      <formula>A29&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B59">
+    <cfRule type="expression" dxfId="34" priority="23">
+      <formula>A59&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B55:B56">
+    <cfRule type="expression" dxfId="33" priority="22">
+      <formula>A55&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B57">
+    <cfRule type="expression" dxfId="32" priority="21">
+      <formula>A57&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B54">
+    <cfRule type="expression" dxfId="31" priority="20">
+      <formula>A54&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B58">
+    <cfRule type="expression" dxfId="30" priority="19">
+      <formula>A58&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B53">
+    <cfRule type="expression" dxfId="29" priority="18">
+      <formula>A53&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B69:B70">
+    <cfRule type="expression" dxfId="28" priority="17">
+      <formula>A69&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B61 B65:B67 B63">
+    <cfRule type="expression" dxfId="27" priority="16">
+      <formula>A61&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B68">
+    <cfRule type="expression" dxfId="26" priority="15">
+      <formula>A68&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B64">
-    <cfRule type="expression" dxfId="49" priority="59">
+    <cfRule type="expression" dxfId="25" priority="14">
       <formula>A64&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B58:B61">
-    <cfRule type="expression" dxfId="48" priority="58">
-      <formula>A58&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B65">
-    <cfRule type="expression" dxfId="47" priority="57">
-      <formula>A65&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="B62">
-    <cfRule type="expression" dxfId="46" priority="56">
+    <cfRule type="expression" dxfId="24" priority="13">
       <formula>A62&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B63">
-    <cfRule type="expression" dxfId="45" priority="55">
-      <formula>A63&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B69">
-    <cfRule type="expression" dxfId="44" priority="54">
-      <formula>A69&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B80">
-    <cfRule type="expression" dxfId="43" priority="53">
-      <formula>A80&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B99">
-    <cfRule type="expression" dxfId="42" priority="52">
-      <formula>A99&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B88:B90 B92">
-    <cfRule type="expression" dxfId="41" priority="51">
-      <formula>A88&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B100">
-    <cfRule type="expression" dxfId="40" priority="50">
-      <formula>A100&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B93">
-    <cfRule type="expression" dxfId="39" priority="49">
-      <formula>A93&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B98">
-    <cfRule type="expression" dxfId="38" priority="48">
-      <formula>A98&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B96">
-    <cfRule type="expression" dxfId="37" priority="47">
-      <formula>A96&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B94">
-    <cfRule type="expression" dxfId="36" priority="45">
-      <formula>A94&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B97">
-    <cfRule type="expression" dxfId="35" priority="44">
-      <formula>A97&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B107">
-    <cfRule type="expression" dxfId="34" priority="43">
-      <formula>A107&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B101:B104">
-    <cfRule type="expression" dxfId="33" priority="42">
-      <formula>A101&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B108">
-    <cfRule type="expression" dxfId="32" priority="41">
-      <formula>A108&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B105">
-    <cfRule type="expression" dxfId="31" priority="40">
-      <formula>A105&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B106">
-    <cfRule type="expression" dxfId="30" priority="39">
-      <formula>A106&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B91">
-    <cfRule type="expression" dxfId="29" priority="38">
-      <formula>A91&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B95">
-    <cfRule type="expression" dxfId="28" priority="37">
-      <formula>A95&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B83">
-    <cfRule type="expression" dxfId="27" priority="34">
-      <formula>A83&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B19:B21">
-    <cfRule type="expression" dxfId="26" priority="33">
-      <formula>A19&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B12:B14">
-    <cfRule type="expression" dxfId="25" priority="32">
-      <formula>A12&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B17">
-    <cfRule type="expression" dxfId="24" priority="31">
-      <formula>A17&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B10">
-    <cfRule type="expression" dxfId="23" priority="29">
-      <formula>A10&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B4:B7">
-    <cfRule type="expression" dxfId="22" priority="28">
-      <formula>A4&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B9">
-    <cfRule type="expression" dxfId="21" priority="26">
-      <formula>A9&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B16">
-    <cfRule type="expression" dxfId="20" priority="25">
-      <formula>A16&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B8">
-    <cfRule type="expression" dxfId="19" priority="24">
-      <formula>A8&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B23:B24">
-    <cfRule type="expression" dxfId="18" priority="21">
-      <formula>A23&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B18">
-    <cfRule type="expression" dxfId="17" priority="18">
-      <formula>A18&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B26">
-    <cfRule type="expression" dxfId="16" priority="17">
-      <formula>A26&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B30:B32">
-    <cfRule type="expression" dxfId="15" priority="16">
-      <formula>A30&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B25">
-    <cfRule type="expression" dxfId="14" priority="15">
-      <formula>A25&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B28">
-    <cfRule type="expression" dxfId="13" priority="14">
-      <formula>A28&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B27">
-    <cfRule type="expression" dxfId="12" priority="13">
-      <formula>A27&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B29">
-    <cfRule type="expression" dxfId="11" priority="12">
-      <formula>A29&lt;&gt;""</formula>
+  <conditionalFormatting sqref="B41 B52">
+    <cfRule type="expression" dxfId="23" priority="12">
+      <formula>A41&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B40">
-    <cfRule type="expression" dxfId="10" priority="11">
+    <cfRule type="expression" dxfId="21" priority="11">
       <formula>A40&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B36:B37">
-    <cfRule type="expression" dxfId="9" priority="10">
+    <cfRule type="expression" dxfId="19" priority="10">
       <formula>A36&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B38">
-    <cfRule type="expression" dxfId="8" priority="9">
+    <cfRule type="expression" dxfId="17" priority="9">
       <formula>A38&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B35">
-    <cfRule type="expression" dxfId="7" priority="8">
+    <cfRule type="expression" dxfId="15" priority="8">
       <formula>A35&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B39">
-    <cfRule type="expression" dxfId="6" priority="7">
+    <cfRule type="expression" dxfId="13" priority="7">
       <formula>A39&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B34">
-    <cfRule type="expression" dxfId="5" priority="6">
+    <cfRule type="expression" dxfId="11" priority="6">
       <formula>A34&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B50:B51">
-    <cfRule type="expression" dxfId="4" priority="5">
+    <cfRule type="expression" dxfId="9" priority="5">
       <formula>A50&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B42 B46:B48 B44">
-    <cfRule type="expression" dxfId="3" priority="4">
+    <cfRule type="expression" dxfId="7" priority="4">
       <formula>A42&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B49">
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="5" priority="3">
       <formula>A49&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B45">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="3" priority="2">
       <formula>A45&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B43">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>A43&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
`todos.completed` date type delete `recors.position`
</commit_message>
<xml_diff>
--- a/db_notebook_definition.xlsx
+++ b/db_notebook_definition.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="85">
   <si>
     <t>登録日</t>
     <rPh sb="0" eb="3">
@@ -982,196 +982,7 @@
     <cellStyle name="標準 2" xfId="4"/>
     <cellStyle name="良い" xfId="6" builtinId="26"/>
   </cellStyles>
-  <dxfs count="85">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="58">
     <dxf>
       <fill>
         <patternFill>
@@ -1588,8 +1399,8 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="テーブル133" displayName="テーブル133" ref="B6:F26" totalsRowShown="0">
   <tableColumns count="5">
-    <tableColumn id="1" name="No." dataDxfId="84"/>
-    <tableColumn id="2" name="テーブル" dataDxfId="83"/>
+    <tableColumn id="1" name="No." dataDxfId="57"/>
+    <tableColumn id="2" name="テーブル" dataDxfId="56"/>
     <tableColumn id="3" name="テーブル名"/>
     <tableColumn id="5" name="インデックス" dataCellStyle="標準 2"/>
     <tableColumn id="4" name="用途"/>
@@ -1883,10 +1694,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I91"/>
+  <dimension ref="A1:I90"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A70" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C82" sqref="C82"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A67" sqref="A67:XFD67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.15"/>
@@ -3004,13 +2815,13 @@
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B67" s="15" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="C67" s="15" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="D67" s="15" t="s">
-        <v>16</v>
+        <v>61</v>
       </c>
       <c r="E67" s="16"/>
       <c r="F67" s="16"/>
@@ -3020,150 +2831,150 @@
       <c r="H67" s="17"/>
       <c r="I67" s="36" t="str">
         <f>IF(A67="","","/* ") &amp; "`" &amp; C67 &amp; "` " &amp; D67 &amp; IF(E67&gt;0,"(" &amp; E67 &amp; ") "," ") &amp; IF(F67&lt;&gt;"","NOT NULL ","") &amp; IF(G67="","","DEFAULT '" &amp; G67 &amp; "' ") &amp; "COMMENT '"&amp; B67 &amp;"'," &amp; IF(A67="",""," */")</f>
-        <v>`position` INT DEFAULT '0' COMMENT 'position',</v>
+        <v>`priority` BOOLEAN DEFAULT '0' COMMENT 'priority',</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A68" s="22"/>
       <c r="B68" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="C68" s="15" t="s">
-        <v>60</v>
+        <v>0</v>
+      </c>
+      <c r="C68" s="18" t="s">
+        <v>10</v>
       </c>
       <c r="D68" s="15" t="s">
-        <v>61</v>
+        <v>11</v>
       </c>
       <c r="E68" s="16"/>
       <c r="F68" s="16"/>
-      <c r="G68" s="16">
-        <v>0</v>
-      </c>
+      <c r="G68" s="16"/>
       <c r="H68" s="17"/>
       <c r="I68" s="36" t="str">
-        <f>IF(A68="","","/* ") &amp; "`" &amp; C68 &amp; "` " &amp; D68 &amp; IF(E68&gt;0,"(" &amp; E68 &amp; ") "," ") &amp; IF(F68&lt;&gt;"","NOT NULL ","") &amp; IF(G68="","","DEFAULT '" &amp; G68 &amp; "' ") &amp; "COMMENT '"&amp; B68 &amp;"'," &amp; IF(A68="",""," */")</f>
-        <v>`priority` BOOLEAN DEFAULT '0' COMMENT 'priority',</v>
+        <f t="shared" ref="I68" si="10">IF(A68="","","/* ") &amp; "`" &amp; C68 &amp; "` " &amp; D68 &amp; IF(E68&gt;0,"(" &amp; E68 &amp; ") "," ") &amp; IF(F68&lt;&gt;"","NOT NULL ","") &amp; IF(G68="","","DEFAULT '" &amp; G68 &amp; "' ") &amp; "COMMENT '"&amp; B68 &amp;"'," &amp; IF(A68="",""," */")</f>
+        <v>`created` DATETIME COMMENT '登録日',</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A69" s="22"/>
-      <c r="B69" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="C69" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="D69" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="E69" s="16"/>
-      <c r="F69" s="16"/>
-      <c r="G69" s="16"/>
-      <c r="H69" s="17"/>
-      <c r="I69" s="36" t="str">
-        <f t="shared" ref="I69" si="10">IF(A69="","","/* ") &amp; "`" &amp; C69 &amp; "` " &amp; D69 &amp; IF(E69&gt;0,"(" &amp; E69 &amp; ") "," ") &amp; IF(F69&lt;&gt;"","NOT NULL ","") &amp; IF(G69="","","DEFAULT '" &amp; G69 &amp; "' ") &amp; "COMMENT '"&amp; B69 &amp;"'," &amp; IF(A69="",""," */")</f>
-        <v>`created` DATETIME COMMENT '登録日',</v>
-      </c>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A70" s="22"/>
-      <c r="I70" s="37" t="s">
+      <c r="I69" s="37" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="71" spans="1:9" s="28" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="A71" s="43"/>
-      <c r="H71" s="29"/>
+    <row r="70" spans="1:9" s="28" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="A70" s="43"/>
+      <c r="H70" s="29"/>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="B71" s="42" t="s">
+        <v>79</v>
+      </c>
+      <c r="D71" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="E71" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="F71" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="G71" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="H71" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="I71" s="30"/>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B72" s="42" t="s">
-        <v>79</v>
-      </c>
-      <c r="D72" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="E72" s="31" t="s">
-        <v>5</v>
-      </c>
-      <c r="F72" s="31" t="s">
-        <v>7</v>
-      </c>
-      <c r="G72" s="31" t="s">
-        <v>8</v>
-      </c>
-      <c r="H72" s="32" t="s">
-        <v>18</v>
-      </c>
-      <c r="I72" s="30"/>
+      <c r="B72" s="51" t="s">
+        <v>82</v>
+      </c>
+      <c r="C72" s="51" t="s">
+        <v>83</v>
+      </c>
+      <c r="D72" s="33"/>
+      <c r="E72" s="34"/>
+      <c r="F72" s="34"/>
+      <c r="G72" s="34"/>
+      <c r="H72" s="35"/>
+      <c r="I72" s="27" t="str">
+        <f xml:space="preserve"> "CREATE TABLE `" &amp; C72 &amp; "` ("</f>
+        <v>CREATE TABLE `calendars` (</v>
+      </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B73" s="51" t="s">
-        <v>82</v>
-      </c>
-      <c r="C73" s="51" t="s">
-        <v>83</v>
-      </c>
-      <c r="D73" s="33"/>
-      <c r="E73" s="34"/>
-      <c r="F73" s="34"/>
-      <c r="G73" s="34"/>
-      <c r="H73" s="35"/>
-      <c r="I73" s="27" t="str">
-        <f xml:space="preserve"> "CREATE TABLE `" &amp; C73 &amp; "` ("</f>
-        <v>CREATE TABLE `calendars` (</v>
+      <c r="B73" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C73" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="D73" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E73" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F73" s="16"/>
+      <c r="G73" s="16"/>
+      <c r="H73" s="17"/>
+      <c r="I73" s="27" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B74" s="15" t="s">
-        <v>9</v>
+        <v>50</v>
       </c>
       <c r="C74" s="15" t="s">
-        <v>1</v>
+        <v>84</v>
       </c>
       <c r="D74" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="E74" s="16" t="s">
-        <v>6</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="E74" s="16"/>
       <c r="F74" s="16"/>
       <c r="G74" s="16"/>
       <c r="H74" s="17"/>
-      <c r="I74" s="27" t="s">
-        <v>3</v>
+      <c r="I74" s="36" t="str">
+        <f t="shared" ref="I74:I81" si="11">IF(A74="","","/* ") &amp; "`" &amp; C74 &amp; "` " &amp; D74 &amp; IF(E74&gt;0,"(" &amp; E74 &amp; ") "," ") &amp; IF(F74&lt;&gt;"","NOT NULL ","") &amp; IF(G74="","","DEFAULT '" &amp; G74 &amp; "' ") &amp; "COMMENT '"&amp; B74 &amp;"'," &amp; IF(A74="",""," */")</f>
+        <v>`calendarcategory_id` INT COMMENT 'calendars',</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B75" s="15" t="s">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="C75" s="15" t="s">
-        <v>84</v>
+        <v>45</v>
       </c>
       <c r="D75" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="E75" s="16"/>
-      <c r="F75" s="16"/>
+        <v>13</v>
+      </c>
+      <c r="E75" s="16">
+        <v>128</v>
+      </c>
+      <c r="F75" s="16" t="s">
+        <v>7</v>
+      </c>
       <c r="G75" s="16"/>
       <c r="H75" s="17"/>
       <c r="I75" s="36" t="str">
-        <f t="shared" ref="I75:I82" si="11">IF(A75="","","/* ") &amp; "`" &amp; C75 &amp; "` " &amp; D75 &amp; IF(E75&gt;0,"(" &amp; E75 &amp; ") "," ") &amp; IF(F75&lt;&gt;"","NOT NULL ","") &amp; IF(G75="","","DEFAULT '" &amp; G75 &amp; "' ") &amp; "COMMENT '"&amp; B75 &amp;"'," &amp; IF(A75="",""," */")</f>
-        <v>`calendarcategory_id` INT COMMENT 'calendars',</v>
+        <f t="shared" si="11"/>
+        <v>`title` VARCHAR(128) NOT NULL COMMENT '名前',</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B76" s="15" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="C76" s="15" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D76" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="E76" s="16">
-        <v>128</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="E76" s="16"/>
       <c r="F76" s="16" t="s">
         <v>7</v>
       </c>
@@ -3171,39 +2982,37 @@
       <c r="H76" s="17"/>
       <c r="I76" s="36" t="str">
         <f t="shared" si="11"/>
-        <v>`title` VARCHAR(128) NOT NULL COMMENT '名前',</v>
+        <v>`start` DATE NOT NULL COMMENT 'dayofevent',</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B77" s="15" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C77" s="15" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D77" s="15" t="s">
         <v>29</v>
       </c>
       <c r="E77" s="16"/>
-      <c r="F77" s="16" t="s">
-        <v>7</v>
-      </c>
+      <c r="F77" s="16"/>
       <c r="G77" s="16"/>
       <c r="H77" s="17"/>
       <c r="I77" s="36" t="str">
         <f t="shared" si="11"/>
-        <v>`start` DATE NOT NULL COMMENT 'dayofevent',</v>
+        <v>`end` DATE COMMENT 'end',</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B78" s="15" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C78" s="15" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="D78" s="15" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="E78" s="16"/>
       <c r="F78" s="16"/>
@@ -3211,34 +3020,36 @@
       <c r="H78" s="17"/>
       <c r="I78" s="36" t="str">
         <f t="shared" si="11"/>
-        <v>`end` DATE COMMENT 'end',</v>
+        <v>`detail` TEXT COMMENT 'detail',</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B79" s="15" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="C79" s="15" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="D79" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="E79" s="16"/>
+        <v>13</v>
+      </c>
+      <c r="E79" s="16">
+        <v>32</v>
+      </c>
       <c r="F79" s="16"/>
       <c r="G79" s="16"/>
       <c r="H79" s="17"/>
       <c r="I79" s="36" t="str">
         <f t="shared" si="11"/>
-        <v>`detail` TEXT COMMENT 'detail',</v>
+        <v>`color` VARCHAR(32) COMMENT 'color',</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B80" s="15" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="C80" s="15" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="D80" s="15" t="s">
         <v>13</v>
@@ -3251,342 +3062,316 @@
       <c r="H80" s="17"/>
       <c r="I80" s="36" t="str">
         <f t="shared" si="11"/>
-        <v>`color` VARCHAR(32) COMMENT 'color',</v>
+        <v>`textcolor` VARCHAR(32) COMMENT 'textcolor',</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A81" s="22"/>
       <c r="B81" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="C81" s="15" t="s">
-        <v>48</v>
+        <v>0</v>
+      </c>
+      <c r="C81" s="18" t="s">
+        <v>10</v>
       </c>
       <c r="D81" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="E81" s="16">
-        <v>32</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="E81" s="16"/>
       <c r="F81" s="16"/>
       <c r="G81" s="16"/>
       <c r="H81" s="17"/>
       <c r="I81" s="36" t="str">
         <f t="shared" si="11"/>
-        <v>`textcolor` VARCHAR(32) COMMENT 'textcolor',</v>
+        <v>`created` DATETIME COMMENT '登録日',</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A82" s="22"/>
-      <c r="B82" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="C82" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="D82" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="E82" s="16"/>
-      <c r="F82" s="16"/>
-      <c r="G82" s="16"/>
-      <c r="H82" s="17"/>
-      <c r="I82" s="36" t="str">
-        <f t="shared" si="11"/>
-        <v>`created` DATETIME COMMENT '登録日',</v>
-      </c>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A83" s="22"/>
-      <c r="I83" s="37" t="s">
+      <c r="I82" s="37" t="s">
         <v>2</v>
       </c>
     </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="B84" s="42"/>
+      <c r="D84" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="E84" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="F84" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="G84" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="H84" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="I84" s="30"/>
+    </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B85" s="42"/>
-      <c r="D85" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="E85" s="31" t="s">
-        <v>5</v>
-      </c>
-      <c r="F85" s="31" t="s">
-        <v>7</v>
-      </c>
-      <c r="G85" s="31" t="s">
-        <v>8</v>
-      </c>
-      <c r="H85" s="32" t="s">
-        <v>18</v>
-      </c>
-      <c r="I85" s="30"/>
+      <c r="B85" s="51" t="s">
+        <v>80</v>
+      </c>
+      <c r="C85" s="51" t="s">
+        <v>81</v>
+      </c>
+      <c r="D85" s="33"/>
+      <c r="E85" s="34"/>
+      <c r="F85" s="34"/>
+      <c r="G85" s="34"/>
+      <c r="H85" s="35"/>
+      <c r="I85" s="27" t="str">
+        <f xml:space="preserve"> "CREATE TABLE `" &amp; C85 &amp; "` ("</f>
+        <v>CREATE TABLE `calendarcategories` (</v>
+      </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B86" s="51" t="s">
-        <v>80</v>
-      </c>
-      <c r="C86" s="51" t="s">
-        <v>81</v>
-      </c>
-      <c r="D86" s="33"/>
-      <c r="E86" s="34"/>
-      <c r="F86" s="34"/>
-      <c r="G86" s="34"/>
-      <c r="H86" s="35"/>
-      <c r="I86" s="27" t="str">
-        <f xml:space="preserve"> "CREATE TABLE `" &amp; C86 &amp; "` ("</f>
-        <v>CREATE TABLE `calendarcategories` (</v>
+      <c r="B86" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C86" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="D86" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E86" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F86" s="16"/>
+      <c r="G86" s="16"/>
+      <c r="H86" s="17"/>
+      <c r="I86" s="27" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B87" s="15" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C87" s="15" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="D87" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="E87" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="F87" s="16"/>
+        <v>13</v>
+      </c>
+      <c r="E87" s="16">
+        <v>128</v>
+      </c>
+      <c r="F87" s="16" t="s">
+        <v>7</v>
+      </c>
       <c r="G87" s="16"/>
       <c r="H87" s="17"/>
-      <c r="I87" s="27" t="s">
-        <v>3</v>
+      <c r="I87" s="36" t="str">
+        <f t="shared" ref="I87:I89" si="12">IF(A87="","","/* ") &amp; "`" &amp; C87 &amp; "` " &amp; D87 &amp; IF(E87&gt;0,"(" &amp; E87 &amp; ") "," ") &amp; IF(F87&lt;&gt;"","NOT NULL ","") &amp; IF(G87="","","DEFAULT '" &amp; G87 &amp; "' ") &amp; "COMMENT '"&amp; B87 &amp;"'," &amp; IF(A87="",""," */")</f>
+        <v>`name` VARCHAR(128) NOT NULL COMMENT '名前',</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B88" s="15" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="C88" s="15" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="D88" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="E88" s="16">
-        <v>128</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="E88" s="16"/>
       <c r="F88" s="16" t="s">
         <v>7</v>
       </c>
       <c r="G88" s="16"/>
       <c r="H88" s="17"/>
       <c r="I88" s="36" t="str">
-        <f t="shared" ref="I88:I90" si="12">IF(A88="","","/* ") &amp; "`" &amp; C88 &amp; "` " &amp; D88 &amp; IF(E88&gt;0,"(" &amp; E88 &amp; ") "," ") &amp; IF(F88&lt;&gt;"","NOT NULL ","") &amp; IF(G88="","","DEFAULT '" &amp; G88 &amp; "' ") &amp; "COMMENT '"&amp; B88 &amp;"'," &amp; IF(A88="",""," */")</f>
-        <v>`name` VARCHAR(128) NOT NULL COMMENT '名前',</v>
+        <f t="shared" si="12"/>
+        <v>`position` INT NOT NULL COMMENT 'position',</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A89" s="22"/>
       <c r="B89" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="C89" s="15" t="s">
-        <v>34</v>
+        <v>0</v>
+      </c>
+      <c r="C89" s="18" t="s">
+        <v>10</v>
       </c>
       <c r="D89" s="15" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="E89" s="16"/>
-      <c r="F89" s="16" t="s">
-        <v>7</v>
-      </c>
+      <c r="F89" s="16"/>
       <c r="G89" s="16"/>
       <c r="H89" s="17"/>
       <c r="I89" s="36" t="str">
         <f t="shared" si="12"/>
-        <v>`position` INT NOT NULL COMMENT 'position',</v>
+        <v>`created` DATETIME COMMENT '登録日',</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A90" s="22"/>
-      <c r="B90" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="C90" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="D90" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="E90" s="16"/>
-      <c r="F90" s="16"/>
-      <c r="G90" s="16"/>
-      <c r="H90" s="17"/>
-      <c r="I90" s="36" t="str">
-        <f t="shared" si="12"/>
-        <v>`created` DATETIME COMMENT '登録日',</v>
-      </c>
-    </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A91" s="22"/>
-      <c r="I91" s="37" t="s">
+      <c r="I90" s="37" t="s">
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="7"/>
-  <conditionalFormatting sqref="B1:B3 B15 B22 B11 B33 B69:B70 B93:B1048576">
-    <cfRule type="expression" dxfId="56" priority="211">
+  <conditionalFormatting sqref="B1:B3 B15 B22 B11 B33 B68:B69 B92:B1048576">
+    <cfRule type="expression" dxfId="55" priority="211">
       <formula>A1&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19:B21">
-    <cfRule type="expression" dxfId="55" priority="82">
+    <cfRule type="expression" dxfId="54" priority="82">
       <formula>A19&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12:B14">
-    <cfRule type="expression" dxfId="54" priority="81">
+    <cfRule type="expression" dxfId="53" priority="81">
       <formula>A12&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17">
-    <cfRule type="expression" dxfId="53" priority="80">
+    <cfRule type="expression" dxfId="52" priority="80">
       <formula>A17&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10">
-    <cfRule type="expression" dxfId="52" priority="78">
+    <cfRule type="expression" dxfId="51" priority="78">
       <formula>A10&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:B7">
-    <cfRule type="expression" dxfId="51" priority="77">
+    <cfRule type="expression" dxfId="50" priority="77">
       <formula>A4&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9">
-    <cfRule type="expression" dxfId="50" priority="75">
+    <cfRule type="expression" dxfId="49" priority="75">
       <formula>A9&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16">
-    <cfRule type="expression" dxfId="49" priority="74">
+    <cfRule type="expression" dxfId="48" priority="74">
       <formula>A16&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8">
-    <cfRule type="expression" dxfId="48" priority="73">
+    <cfRule type="expression" dxfId="47" priority="73">
       <formula>A8&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23:B24">
-    <cfRule type="expression" dxfId="47" priority="70">
+    <cfRule type="expression" dxfId="46" priority="70">
       <formula>A23&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18">
-    <cfRule type="expression" dxfId="46" priority="67">
+    <cfRule type="expression" dxfId="45" priority="67">
       <formula>A18&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B26">
-    <cfRule type="expression" dxfId="45" priority="66">
+    <cfRule type="expression" dxfId="44" priority="66">
       <formula>A26&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B30:B32">
-    <cfRule type="expression" dxfId="44" priority="65">
+    <cfRule type="expression" dxfId="43" priority="65">
       <formula>A30&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B25">
-    <cfRule type="expression" dxfId="43" priority="64">
+    <cfRule type="expression" dxfId="42" priority="64">
       <formula>A25&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B28">
-    <cfRule type="expression" dxfId="42" priority="63">
+    <cfRule type="expression" dxfId="41" priority="63">
       <formula>A28&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B27">
-    <cfRule type="expression" dxfId="41" priority="62">
+    <cfRule type="expression" dxfId="40" priority="62">
       <formula>A27&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B29">
-    <cfRule type="expression" dxfId="40" priority="61">
+    <cfRule type="expression" dxfId="39" priority="61">
       <formula>A29&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B41 B52">
-    <cfRule type="expression" dxfId="39" priority="49">
+    <cfRule type="expression" dxfId="38" priority="49">
       <formula>A41&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B40">
-    <cfRule type="expression" dxfId="38" priority="48">
+    <cfRule type="expression" dxfId="37" priority="48">
       <formula>A40&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B36:B37">
-    <cfRule type="expression" dxfId="37" priority="47">
+    <cfRule type="expression" dxfId="36" priority="47">
       <formula>A36&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B38">
-    <cfRule type="expression" dxfId="36" priority="46">
+    <cfRule type="expression" dxfId="35" priority="46">
       <formula>A38&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B35">
-    <cfRule type="expression" dxfId="35" priority="45">
+    <cfRule type="expression" dxfId="34" priority="45">
       <formula>A35&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B39">
-    <cfRule type="expression" dxfId="34" priority="44">
+    <cfRule type="expression" dxfId="33" priority="44">
       <formula>A39&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B34">
-    <cfRule type="expression" dxfId="33" priority="43">
+    <cfRule type="expression" dxfId="32" priority="43">
       <formula>A34&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B50:B51">
-    <cfRule type="expression" dxfId="32" priority="42">
+    <cfRule type="expression" dxfId="31" priority="42">
       <formula>A50&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B42 B46:B48 B44">
-    <cfRule type="expression" dxfId="31" priority="41">
+    <cfRule type="expression" dxfId="30" priority="41">
       <formula>A42&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B49">
-    <cfRule type="expression" dxfId="30" priority="40">
+    <cfRule type="expression" dxfId="29" priority="40">
       <formula>A49&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B45">
-    <cfRule type="expression" dxfId="29" priority="39">
+    <cfRule type="expression" dxfId="28" priority="39">
       <formula>A45&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B43">
-    <cfRule type="expression" dxfId="28" priority="38">
+    <cfRule type="expression" dxfId="27" priority="38">
       <formula>A43&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B66 B71 B60">
-    <cfRule type="expression" dxfId="27" priority="37">
+  <conditionalFormatting sqref="B66 B70 B60">
+    <cfRule type="expression" dxfId="26" priority="37">
       <formula>A60&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B61:B63">
-    <cfRule type="expression" dxfId="26" priority="35">
+    <cfRule type="expression" dxfId="25" priority="35">
       <formula>A61&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B67">
-    <cfRule type="expression" dxfId="25" priority="34">
-      <formula>A67&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B59">
@@ -3614,9 +3399,9 @@
       <formula>A57&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B68">
+  <conditionalFormatting sqref="B67">
     <cfRule type="expression" dxfId="19" priority="28">
-      <formula>A68&lt;&gt;""</formula>
+      <formula>A67&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B65">
@@ -3624,94 +3409,94 @@
       <formula>A65&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="B82">
+    <cfRule type="expression" dxfId="17" priority="21">
+      <formula>A82&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B75 B73">
+    <cfRule type="expression" dxfId="16" priority="20">
+      <formula>A73&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="B83">
-    <cfRule type="expression" dxfId="17" priority="21">
+    <cfRule type="expression" dxfId="15" priority="19">
       <formula>A83&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B76 B74">
-    <cfRule type="expression" dxfId="16" priority="20">
+  <conditionalFormatting sqref="B76">
+    <cfRule type="expression" dxfId="14" priority="18">
+      <formula>A76&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B81">
+    <cfRule type="expression" dxfId="13" priority="17">
+      <formula>A81&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B79">
+    <cfRule type="expression" dxfId="12" priority="16">
+      <formula>A79&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B77">
+    <cfRule type="expression" dxfId="11" priority="15">
+      <formula>A77&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B80">
+    <cfRule type="expression" dxfId="10" priority="14">
+      <formula>A80&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B74">
+    <cfRule type="expression" dxfId="9" priority="13">
       <formula>A74&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B84">
-    <cfRule type="expression" dxfId="15" priority="19">
+  <conditionalFormatting sqref="B78">
+    <cfRule type="expression" dxfId="8" priority="12">
+      <formula>A78&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B71">
+    <cfRule type="expression" dxfId="7" priority="8">
+      <formula>A71&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B72">
+    <cfRule type="expression" dxfId="6" priority="9">
+      <formula>A72&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B90">
+    <cfRule type="expression" dxfId="5" priority="7">
+      <formula>A90&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B84 B86:B87">
+    <cfRule type="expression" dxfId="4" priority="6">
       <formula>A84&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B77">
-    <cfRule type="expression" dxfId="14" priority="18">
-      <formula>A77&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B82">
-    <cfRule type="expression" dxfId="13" priority="17">
-      <formula>A82&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B80">
-    <cfRule type="expression" dxfId="12" priority="16">
-      <formula>A80&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B78">
-    <cfRule type="expression" dxfId="11" priority="15">
-      <formula>A78&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B81">
-    <cfRule type="expression" dxfId="10" priority="14">
-      <formula>A81&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B75">
-    <cfRule type="expression" dxfId="9" priority="13">
-      <formula>A75&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B79">
-    <cfRule type="expression" dxfId="8" priority="12">
-      <formula>A79&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B72">
-    <cfRule type="expression" dxfId="7" priority="8">
-      <formula>A72&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B73">
-    <cfRule type="expression" dxfId="6" priority="9">
-      <formula>A73&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="B91">
-    <cfRule type="expression" dxfId="5" priority="7">
+    <cfRule type="expression" dxfId="3" priority="5">
       <formula>A91&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B85 B87:B88">
-    <cfRule type="expression" dxfId="4" priority="6">
+  <conditionalFormatting sqref="B88">
+    <cfRule type="expression" dxfId="2" priority="4">
+      <formula>A88&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B89">
+    <cfRule type="expression" dxfId="1" priority="3">
+      <formula>A89&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B85">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>A85&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B92">
-    <cfRule type="expression" dxfId="3" priority="5">
-      <formula>A92&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B89">
-    <cfRule type="expression" dxfId="2" priority="4">
-      <formula>A89&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B90">
-    <cfRule type="expression" dxfId="1" priority="3">
-      <formula>A90&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B86">
-    <cfRule type="expression" dxfId="0" priority="1">
-      <formula>A86&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
holidays from google calendar
</commit_message>
<xml_diff>
--- a/db_notebook_definition.xlsx
+++ b/db_notebook_definition.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="119">
   <si>
     <t>登録日</t>
     <rPh sb="0" eb="3">
@@ -547,6 +547,33 @@
   </si>
   <si>
     <t>5,2</t>
+    <phoneticPr fontId="7"/>
+  </si>
+  <si>
+    <t>holiday</t>
+    <phoneticPr fontId="7"/>
+  </si>
+  <si>
+    <t>holidays</t>
+    <phoneticPr fontId="7"/>
+  </si>
+  <si>
+    <t>変更日</t>
+    <rPh sb="0" eb="3">
+      <t>ヘンコウビ</t>
+    </rPh>
+    <phoneticPr fontId="7"/>
+  </si>
+  <si>
+    <t>modified</t>
+    <phoneticPr fontId="7"/>
+  </si>
+  <si>
+    <t>DATETIME</t>
+    <phoneticPr fontId="7"/>
+  </si>
+  <si>
+    <t>day</t>
     <phoneticPr fontId="7"/>
   </si>
 </sst>
@@ -1105,7 +1132,707 @@
     <cellStyle name="標準 2" xfId="4"/>
     <cellStyle name="良い" xfId="6" builtinId="26"/>
   </cellStyles>
-  <dxfs count="87">
+  <dxfs count="102">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -1113,601 +1840,6 @@
     </dxf>
     <dxf>
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1725,8 +1857,8 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="テーブル133" displayName="テーブル133" ref="B6:F26" totalsRowShown="0">
   <tableColumns count="5">
-    <tableColumn id="1" name="No." dataDxfId="1"/>
-    <tableColumn id="2" name="テーブル" dataDxfId="0"/>
+    <tableColumn id="1" name="No." dataDxfId="101"/>
+    <tableColumn id="2" name="テーブル" dataDxfId="100"/>
     <tableColumn id="3" name="テーブル名"/>
     <tableColumn id="5" name="インデックス" dataCellStyle="標準 2"/>
     <tableColumn id="4" name="用途"/>
@@ -2020,10 +2152,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J131"/>
+  <dimension ref="A1:J140"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A103" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F116" sqref="F116"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A82" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D104" sqref="D104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.15"/>
@@ -4012,9 +4144,7 @@
       </c>
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B100" s="42" t="s">
-        <v>94</v>
-      </c>
+      <c r="B100" s="42"/>
       <c r="D100" s="30" t="s">
         <v>4</v>
       </c>
@@ -4035,10 +4165,10 @@
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.15">
       <c r="B101" s="51" t="s">
-        <v>95</v>
+        <v>113</v>
       </c>
       <c r="C101" s="51" t="s">
-        <v>96</v>
+        <v>114</v>
       </c>
       <c r="D101" s="33"/>
       <c r="E101" s="34"/>
@@ -4047,11 +4177,11 @@
       <c r="H101" s="35"/>
       <c r="I101" s="27" t="str">
         <f xml:space="preserve"> "CREATE TABLE `" &amp; C101 &amp; "` ("</f>
-        <v>CREATE TABLE `timelogcategories` (</v>
+        <v>CREATE TABLE `holidays` (</v>
       </c>
       <c r="J101" s="27" t="str">
         <f xml:space="preserve"> "CREATE TABLE `" &amp; C101 &amp; "` ("</f>
-        <v>CREATE TABLE `timelogcategories` (</v>
+        <v>CREATE TABLE `holidays` (</v>
       </c>
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.15">
@@ -4088,7 +4218,7 @@
         <v>13</v>
       </c>
       <c r="E103" s="16">
-        <v>128</v>
+        <v>64</v>
       </c>
       <c r="F103" s="16" t="s">
         <v>7</v>
@@ -4096,39 +4226,37 @@
       <c r="G103" s="16"/>
       <c r="H103" s="17"/>
       <c r="I103" s="36" t="str">
-        <f t="shared" ref="I103" si="26">IF(A103="","","/* ") &amp; "`" &amp; C103 &amp; "` " &amp; D103 &amp; IF(E103&gt;0,"(" &amp; E103 &amp; ") "," ") &amp; IF(F103&lt;&gt;"","NOT NULL ","") &amp; IF(G103="","","DEFAULT '" &amp; G103 &amp; "' ") &amp; "COMMENT '"&amp; B103 &amp;"'," &amp; IF(A103="",""," */")</f>
-        <v>`name` VARCHAR(128) NOT NULL COMMENT '名前',</v>
+        <f t="shared" ref="I103:I106" si="26">IF(A103="","","/* ") &amp; "`" &amp; C103 &amp; "` " &amp; D103 &amp; IF(E103&gt;0,"(" &amp; E103 &amp; ") "," ") &amp; IF(F103&lt;&gt;"","NOT NULL ","") &amp; IF(G103="","","DEFAULT '" &amp; G103 &amp; "' ") &amp; "COMMENT '"&amp; B103 &amp;"'," &amp; IF(A103="",""," */")</f>
+        <v>`name` VARCHAR(64) NOT NULL COMMENT '名前',</v>
       </c>
       <c r="J103" s="36" t="str">
-        <f t="shared" ref="J103:J107" si="27">"," &amp;  "`" &amp; C103 &amp; "` " &amp; D103 &amp; IF(E103&gt;0,"(" &amp; E103 &amp; ") "," ") &amp; IF(F103&lt;&gt;"","NOT NULL ","") &amp; IF(G103="","","DEFAULT '" &amp; G103 &amp; "' ")</f>
-        <v xml:space="preserve">,`name` VARCHAR(128) NOT NULL </v>
+        <f>"," &amp;  "`" &amp; C103 &amp; "` " &amp; D103 &amp; IF(E103&gt;0,"(" &amp; E103 &amp; ") "," ") &amp; IF(F103&lt;&gt;"","NOT NULL ","") &amp; IF(G103="","","DEFAULT '" &amp; G103 &amp; "' ")</f>
+        <v xml:space="preserve">,`name` VARCHAR(64) NOT NULL </v>
       </c>
     </row>
     <row r="104" spans="1:10" x14ac:dyDescent="0.15">
       <c r="B104" s="15" t="s">
-        <v>34</v>
+        <v>118</v>
       </c>
       <c r="C104" s="15" t="s">
-        <v>58</v>
+        <v>118</v>
       </c>
       <c r="D104" s="15" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="E104" s="16"/>
       <c r="F104" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="G104" s="16">
-        <v>0</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="G104" s="16"/>
       <c r="H104" s="17"/>
       <c r="I104" s="36" t="str">
-        <f>IF(A104="","","/* ") &amp; "`" &amp; C104 &amp; "` " &amp; D104 &amp; IF(E104&gt;0,"(" &amp; E104 &amp; ") "," ") &amp; IF(F104&lt;&gt;"","NOT NULL ","") &amp; IF(G104="","","DEFAULT '" &amp; G104 &amp; "' ") &amp; "COMMENT '"&amp; B104 &amp;"'," &amp; IF(A104="",""," */")</f>
-        <v>`position` INT NOT NULL DEFAULT '0' COMMENT 'position',</v>
+        <f t="shared" si="26"/>
+        <v>`day` DATE NOT NULL COMMENT 'day',</v>
       </c>
       <c r="J104" s="36" t="str">
-        <f t="shared" si="27"/>
-        <v xml:space="preserve">,`position` INT NOT NULL DEFAULT '0' </v>
+        <f t="shared" ref="J104:J106" si="27">"," &amp;  "`" &amp; C104 &amp; "` " &amp; D104 &amp; IF(E104&gt;0,"(" &amp; E104 &amp; ") "," ") &amp; IF(F104&lt;&gt;"","NOT NULL ","") &amp; IF(G104="","","DEFAULT '" &amp; G104 &amp; "' ")</f>
+        <v xml:space="preserve">,`day` DATE NOT NULL </v>
       </c>
     </row>
     <row r="105" spans="1:10" x14ac:dyDescent="0.15">
@@ -4147,7 +4275,7 @@
       <c r="G105" s="16"/>
       <c r="H105" s="17"/>
       <c r="I105" s="36" t="str">
-        <f t="shared" ref="I105:I107" si="28">IF(A105="","","/* ") &amp; "`" &amp; C105 &amp; "` " &amp; D105 &amp; IF(E105&gt;0,"(" &amp; E105 &amp; ") "," ") &amp; IF(F105&lt;&gt;"","NOT NULL ","") &amp; IF(G105="","","DEFAULT '" &amp; G105 &amp; "' ") &amp; "COMMENT '"&amp; B105 &amp;"'," &amp; IF(A105="",""," */")</f>
+        <f t="shared" si="26"/>
         <v>`created` DATETIME COMMENT '登録日',</v>
       </c>
       <c r="J105" s="36" t="str">
@@ -4158,391 +4286,391 @@
     <row r="106" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A106" s="22"/>
       <c r="B106" s="15" t="s">
-        <v>98</v>
+        <v>115</v>
       </c>
       <c r="C106" s="18" t="s">
-        <v>89</v>
+        <v>116</v>
       </c>
       <c r="D106" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="E106" s="16">
-        <v>4</v>
-      </c>
+        <v>117</v>
+      </c>
+      <c r="E106" s="16"/>
       <c r="F106" s="16"/>
-      <c r="G106" s="16">
-        <v>0</v>
-      </c>
+      <c r="G106" s="16"/>
       <c r="H106" s="17"/>
       <c r="I106" s="36" t="str">
-        <f t="shared" si="28"/>
-        <v>`deleted` TINYINT(4) DEFAULT '0' COMMENT '削除フラグ',</v>
+        <f t="shared" si="26"/>
+        <v>`modified` DATETIME COMMENT '変更日',</v>
       </c>
       <c r="J106" s="36" t="str">
         <f t="shared" si="27"/>
-        <v xml:space="preserve">,`deleted` TINYINT(4) DEFAULT '0' </v>
+        <v xml:space="preserve">,`modified` DATETIME </v>
       </c>
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A107" s="22"/>
-      <c r="B107" s="15" t="s">
-        <v>99</v>
-      </c>
-      <c r="C107" s="18" t="s">
-        <v>90</v>
-      </c>
-      <c r="D107" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="E107" s="16"/>
-      <c r="F107" s="16"/>
-      <c r="G107" s="16"/>
-      <c r="H107" s="17"/>
-      <c r="I107" s="36" t="str">
-        <f t="shared" si="28"/>
-        <v>`deleted_date` DATETIME COMMENT '削除日',</v>
-      </c>
-      <c r="J107" s="36" t="str">
-        <f t="shared" si="27"/>
-        <v xml:space="preserve">,`deleted_date` DATETIME </v>
-      </c>
-    </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A108" s="22"/>
-      <c r="I108" s="37" t="s">
+      <c r="I107" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="J108" s="37" t="s">
+      <c r="J107" s="37" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="109" spans="1:10" s="28" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="A109" s="43"/>
-      <c r="H109" s="29"/>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="B109" s="42" t="s">
+        <v>94</v>
+      </c>
+      <c r="D109" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="E109" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="F109" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="G109" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="H109" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="I109" s="30"/>
+      <c r="J109" s="30"/>
     </row>
     <row r="110" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="D110" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="E110" s="31" t="s">
-        <v>5</v>
-      </c>
-      <c r="F110" s="31" t="s">
-        <v>7</v>
-      </c>
-      <c r="G110" s="31" t="s">
-        <v>8</v>
-      </c>
-      <c r="H110" s="32" t="s">
-        <v>18</v>
-      </c>
-      <c r="I110" s="30"/>
-      <c r="J110" s="30"/>
+      <c r="B110" s="51" t="s">
+        <v>95</v>
+      </c>
+      <c r="C110" s="51" t="s">
+        <v>96</v>
+      </c>
+      <c r="D110" s="33"/>
+      <c r="E110" s="34"/>
+      <c r="F110" s="34"/>
+      <c r="G110" s="34"/>
+      <c r="H110" s="35"/>
+      <c r="I110" s="27" t="str">
+        <f xml:space="preserve"> "CREATE TABLE `" &amp; C110 &amp; "` ("</f>
+        <v>CREATE TABLE `timelogcategories` (</v>
+      </c>
+      <c r="J110" s="27" t="str">
+        <f xml:space="preserve"> "CREATE TABLE `" &amp; C110 &amp; "` ("</f>
+        <v>CREATE TABLE `timelogcategories` (</v>
+      </c>
     </row>
     <row r="111" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B111" s="51" t="s">
-        <v>93</v>
-      </c>
-      <c r="C111" s="51" t="s">
-        <v>97</v>
-      </c>
-      <c r="D111" s="33"/>
-      <c r="E111" s="34"/>
-      <c r="F111" s="34"/>
-      <c r="G111" s="34"/>
-      <c r="H111" s="35"/>
-      <c r="I111" s="27" t="str">
-        <f xml:space="preserve"> "CREATE TABLE `" &amp; C111 &amp; "` ("</f>
-        <v>CREATE TABLE `timelogs` (</v>
-      </c>
-      <c r="J111" s="27" t="str">
-        <f xml:space="preserve"> "CREATE TABLE `" &amp; C111 &amp; "` ("</f>
-        <v>CREATE TABLE `timelogs` (</v>
+      <c r="B111" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C111" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="D111" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E111" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F111" s="16"/>
+      <c r="G111" s="16"/>
+      <c r="H111" s="17"/>
+      <c r="I111" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="J111" s="27" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="112" spans="1:10" x14ac:dyDescent="0.15">
       <c r="B112" s="15" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C112" s="15" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="D112" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="E112" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="F112" s="16"/>
+        <v>13</v>
+      </c>
+      <c r="E112" s="16">
+        <v>128</v>
+      </c>
+      <c r="F112" s="16" t="s">
+        <v>7</v>
+      </c>
       <c r="G112" s="16"/>
       <c r="H112" s="17"/>
-      <c r="I112" s="27" t="s">
-        <v>3</v>
-      </c>
-      <c r="J112" s="27" t="s">
-        <v>87</v>
+      <c r="I112" s="36" t="str">
+        <f t="shared" ref="I112" si="28">IF(A112="","","/* ") &amp; "`" &amp; C112 &amp; "` " &amp; D112 &amp; IF(E112&gt;0,"(" &amp; E112 &amp; ") "," ") &amp; IF(F112&lt;&gt;"","NOT NULL ","") &amp; IF(G112="","","DEFAULT '" &amp; G112 &amp; "' ") &amp; "COMMENT '"&amp; B112 &amp;"'," &amp; IF(A112="",""," */")</f>
+        <v>`name` VARCHAR(128) NOT NULL COMMENT '名前',</v>
+      </c>
+      <c r="J112" s="36" t="str">
+        <f t="shared" ref="J112:J116" si="29">"," &amp;  "`" &amp; C112 &amp; "` " &amp; D112 &amp; IF(E112&gt;0,"(" &amp; E112 &amp; ") "," ") &amp; IF(F112&lt;&gt;"","NOT NULL ","") &amp; IF(G112="","","DEFAULT '" &amp; G112 &amp; "' ")</f>
+        <v xml:space="preserve">,`name` VARCHAR(128) NOT NULL </v>
       </c>
     </row>
     <row r="113" spans="1:10" x14ac:dyDescent="0.15">
       <c r="B113" s="15" t="s">
-        <v>56</v>
+        <v>34</v>
       </c>
       <c r="C113" s="15" t="s">
-        <v>100</v>
+        <v>58</v>
       </c>
       <c r="D113" s="15" t="s">
         <v>16</v>
       </c>
       <c r="E113" s="16"/>
-      <c r="F113" s="16"/>
-      <c r="G113" s="16"/>
+      <c r="F113" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="G113" s="16">
+        <v>0</v>
+      </c>
       <c r="H113" s="17"/>
       <c r="I113" s="36" t="str">
         <f>IF(A113="","","/* ") &amp; "`" &amp; C113 &amp; "` " &amp; D113 &amp; IF(E113&gt;0,"(" &amp; E113 &amp; ") "," ") &amp; IF(F113&lt;&gt;"","NOT NULL ","") &amp; IF(G113="","","DEFAULT '" &amp; G113 &amp; "' ") &amp; "COMMENT '"&amp; B113 &amp;"'," &amp; IF(A113="",""," */")</f>
-        <v>`timelogcategory_id` INT COMMENT 'カテゴリ',</v>
+        <v>`position` INT NOT NULL DEFAULT '0' COMMENT 'position',</v>
       </c>
       <c r="J113" s="36" t="str">
-        <f t="shared" ref="J113:J118" si="29">"," &amp;  "`" &amp; C113 &amp; "` " &amp; D113 &amp; IF(E113&gt;0,"(" &amp; E113 &amp; ") "," ") &amp; IF(F113&lt;&gt;"","NOT NULL ","") &amp; IF(G113="","","DEFAULT '" &amp; G113 &amp; "' ")</f>
-        <v xml:space="preserve">,`timelogcategory_id` INT </v>
+        <f t="shared" si="29"/>
+        <v xml:space="preserve">,`position` INT NOT NULL DEFAULT '0' </v>
       </c>
     </row>
     <row r="114" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A114" s="22"/>
       <c r="B114" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="C114" s="15" t="s">
-        <v>108</v>
+        <v>0</v>
+      </c>
+      <c r="C114" s="18" t="s">
+        <v>10</v>
       </c>
       <c r="D114" s="15" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="E114" s="16"/>
       <c r="F114" s="16"/>
       <c r="G114" s="16"/>
       <c r="H114" s="17"/>
       <c r="I114" s="36" t="str">
-        <f>IF(A114="","","/* ") &amp; "`" &amp; C114 &amp; "` " &amp; D114 &amp; IF(E114&gt;0,"(" &amp; E114 &amp; ") "," ") &amp; IF(F114&lt;&gt;"","NOT NULL ","") &amp; IF(G114="","","DEFAULT '" &amp; G114 &amp; "' ") &amp; "COMMENT '"&amp; B114 &amp;"'," &amp; IF(A114="",""," */")</f>
-        <v>`timelogtask_id` INT COMMENT 'タスク',</v>
+        <f t="shared" ref="I114:I116" si="30">IF(A114="","","/* ") &amp; "`" &amp; C114 &amp; "` " &amp; D114 &amp; IF(E114&gt;0,"(" &amp; E114 &amp; ") "," ") &amp; IF(F114&lt;&gt;"","NOT NULL ","") &amp; IF(G114="","","DEFAULT '" &amp; G114 &amp; "' ") &amp; "COMMENT '"&amp; B114 &amp;"'," &amp; IF(A114="",""," */")</f>
+        <v>`created` DATETIME COMMENT '登録日',</v>
       </c>
       <c r="J114" s="36" t="str">
-        <f t="shared" ref="J114" si="30">"," &amp;  "`" &amp; C114 &amp; "` " &amp; D114 &amp; IF(E114&gt;0,"(" &amp; E114 &amp; ") "," ") &amp; IF(F114&lt;&gt;"","NOT NULL ","") &amp; IF(G114="","","DEFAULT '" &amp; G114 &amp; "' ")</f>
-        <v xml:space="preserve">,`timelogtask_id` INT </v>
+        <f t="shared" si="29"/>
+        <v xml:space="preserve">,`created` DATETIME </v>
       </c>
     </row>
     <row r="115" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A115" s="22"/>
       <c r="B115" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="C115" s="15" t="s">
-        <v>102</v>
+        <v>98</v>
+      </c>
+      <c r="C115" s="18" t="s">
+        <v>89</v>
       </c>
       <c r="D115" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="E115" s="16"/>
-      <c r="F115" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="G115" s="16"/>
+        <v>91</v>
+      </c>
+      <c r="E115" s="16">
+        <v>4</v>
+      </c>
+      <c r="F115" s="16"/>
+      <c r="G115" s="16">
+        <v>0</v>
+      </c>
       <c r="H115" s="17"/>
       <c r="I115" s="36" t="str">
-        <f t="shared" ref="I115:I117" si="31">IF(A115="","","/* ") &amp; "`" &amp; C115 &amp; "` " &amp; D115 &amp; IF(E115&gt;0,"(" &amp; E115 &amp; ") "," ") &amp; IF(F115&lt;&gt;"","NOT NULL ","") &amp; IF(G115="","","DEFAULT '" &amp; G115 &amp; "' ") &amp; "COMMENT '"&amp; B115 &amp;"'," &amp; IF(A115="",""," */")</f>
-        <v>`workdate` DATE NOT NULL COMMENT '日付',</v>
+        <f t="shared" si="30"/>
+        <v>`deleted` TINYINT(4) DEFAULT '0' COMMENT '削除フラグ',</v>
       </c>
       <c r="J115" s="36" t="str">
         <f t="shared" si="29"/>
-        <v xml:space="preserve">,`workdate` DATE NOT NULL </v>
+        <v xml:space="preserve">,`deleted` TINYINT(4) DEFAULT '0' </v>
       </c>
     </row>
     <row r="116" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A116" s="22"/>
       <c r="B116" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="C116" s="15" t="s">
-        <v>110</v>
+        <v>99</v>
+      </c>
+      <c r="C116" s="18" t="s">
+        <v>90</v>
       </c>
       <c r="D116" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="E116" s="16" t="s">
-        <v>112</v>
-      </c>
-      <c r="F116" s="16" t="s">
-        <v>7</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="E116" s="16"/>
+      <c r="F116" s="16"/>
       <c r="G116" s="16"/>
       <c r="H116" s="17"/>
       <c r="I116" s="36" t="str">
-        <f t="shared" ref="I116" si="32">IF(A116="","","/* ") &amp; "`" &amp; C116 &amp; "` " &amp; D116 &amp; IF(E116&gt;0,"(" &amp; E116 &amp; ") "," ") &amp; IF(F116&lt;&gt;"","NOT NULL ","") &amp; IF(G116="","","DEFAULT '" &amp; G116 &amp; "' ") &amp; "COMMENT '"&amp; B116 &amp;"'," &amp; IF(A116="",""," */")</f>
-        <v>`worktime` DECIMAL(5,2) NOT NULL COMMENT '時間',</v>
+        <f t="shared" si="30"/>
+        <v>`deleted_date` DATETIME COMMENT '削除日',</v>
       </c>
       <c r="J116" s="36" t="str">
-        <f t="shared" ref="J116" si="33">"," &amp;  "`" &amp; C116 &amp; "` " &amp; D116 &amp; IF(E116&gt;0,"(" &amp; E116 &amp; ") "," ") &amp; IF(F116&lt;&gt;"","NOT NULL ","") &amp; IF(G116="","","DEFAULT '" &amp; G116 &amp; "' ")</f>
-        <v xml:space="preserve">,`worktime` DECIMAL(5,2) NOT NULL </v>
+        <f t="shared" si="29"/>
+        <v xml:space="preserve">,`deleted_date` DATETIME </v>
       </c>
     </row>
     <row r="117" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B117" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="C117" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="D117" s="15" t="s">
-        <v>103</v>
-      </c>
-      <c r="E117" s="16">
-        <v>256</v>
-      </c>
-      <c r="F117" s="16"/>
-      <c r="G117" s="16"/>
-      <c r="H117" s="17"/>
-      <c r="I117" s="36" t="str">
-        <f t="shared" si="31"/>
-        <v>`title` VARCHAR(256) COMMENT '名前',</v>
-      </c>
-      <c r="J117" s="36" t="str">
-        <f t="shared" si="29"/>
-        <v xml:space="preserve">,`title` VARCHAR(256) </v>
-      </c>
-    </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A118" s="22"/>
-      <c r="B118" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="C118" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="D118" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="E118" s="16"/>
-      <c r="F118" s="16"/>
-      <c r="G118" s="16"/>
-      <c r="H118" s="17"/>
-      <c r="I118" s="36" t="str">
-        <f t="shared" ref="I118" si="34">IF(A118="","","/* ") &amp; "`" &amp; C118 &amp; "` " &amp; D118 &amp; IF(E118&gt;0,"(" &amp; E118 &amp; ") "," ") &amp; IF(F118&lt;&gt;"","NOT NULL ","") &amp; IF(G118="","","DEFAULT '" &amp; G118 &amp; "' ") &amp; "COMMENT '"&amp; B118 &amp;"'," &amp; IF(A118="",""," */")</f>
-        <v>`created` DATETIME COMMENT '登録日',</v>
-      </c>
-      <c r="J118" s="36" t="str">
-        <f t="shared" si="29"/>
-        <v xml:space="preserve">,`created` DATETIME </v>
-      </c>
+      <c r="A117" s="22"/>
+      <c r="I117" s="37" t="s">
+        <v>2</v>
+      </c>
+      <c r="J117" s="37" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10" s="28" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="A118" s="43"/>
+      <c r="H118" s="29"/>
     </row>
     <row r="119" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A119" s="22"/>
-      <c r="B119" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="C119" s="18" t="s">
-        <v>105</v>
-      </c>
-      <c r="D119" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="E119" s="16"/>
-      <c r="F119" s="16"/>
-      <c r="G119" s="16"/>
-      <c r="H119" s="17"/>
-      <c r="I119" s="36" t="str">
-        <f t="shared" ref="I119" si="35">IF(A119="","","/* ") &amp; "`" &amp; C119 &amp; "` " &amp; D119 &amp; IF(E119&gt;0,"(" &amp; E119 &amp; ") "," ") &amp; IF(F119&lt;&gt;"","NOT NULL ","") &amp; IF(G119="","","DEFAULT '" &amp; G119 &amp; "' ") &amp; "COMMENT '"&amp; B119 &amp;"'," &amp; IF(A119="",""," */")</f>
-        <v>`modified` DATETIME COMMENT '変更日',</v>
-      </c>
-      <c r="J119" s="36" t="str">
-        <f t="shared" ref="J119" si="36">"," &amp;  "`" &amp; C119 &amp; "` " &amp; D119 &amp; IF(E119&gt;0,"(" &amp; E119 &amp; ") "," ") &amp; IF(F119&lt;&gt;"","NOT NULL ","") &amp; IF(G119="","","DEFAULT '" &amp; G119 &amp; "' ")</f>
-        <v xml:space="preserve">,`modified` DATETIME </v>
-      </c>
+      <c r="D119" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="E119" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="F119" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="G119" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="H119" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="I119" s="30"/>
+      <c r="J119" s="30"/>
     </row>
     <row r="120" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A120" s="22"/>
-      <c r="I120" s="37" t="s">
-        <v>2</v>
-      </c>
-      <c r="J120" s="37" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="121" spans="1:10" s="28" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="A121" s="43"/>
-      <c r="H121" s="29"/>
+      <c r="B120" s="51" t="s">
+        <v>93</v>
+      </c>
+      <c r="C120" s="51" t="s">
+        <v>97</v>
+      </c>
+      <c r="D120" s="33"/>
+      <c r="E120" s="34"/>
+      <c r="F120" s="34"/>
+      <c r="G120" s="34"/>
+      <c r="H120" s="35"/>
+      <c r="I120" s="27" t="str">
+        <f xml:space="preserve"> "CREATE TABLE `" &amp; C120 &amp; "` ("</f>
+        <v>CREATE TABLE `timelogs` (</v>
+      </c>
+      <c r="J120" s="27" t="str">
+        <f xml:space="preserve"> "CREATE TABLE `" &amp; C120 &amp; "` ("</f>
+        <v>CREATE TABLE `timelogs` (</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="B121" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C121" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="D121" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E121" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F121" s="16"/>
+      <c r="G121" s="16"/>
+      <c r="H121" s="17"/>
+      <c r="I121" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="J121" s="27" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="122" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B122" s="42"/>
-      <c r="D122" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="E122" s="31" t="s">
-        <v>5</v>
-      </c>
-      <c r="F122" s="31" t="s">
-        <v>7</v>
-      </c>
-      <c r="G122" s="31" t="s">
-        <v>8</v>
-      </c>
-      <c r="H122" s="32" t="s">
-        <v>18</v>
-      </c>
-      <c r="I122" s="30"/>
-      <c r="J122" s="30"/>
+      <c r="B122" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="C122" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="D122" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="E122" s="16"/>
+      <c r="F122" s="16"/>
+      <c r="G122" s="16"/>
+      <c r="H122" s="17"/>
+      <c r="I122" s="36" t="str">
+        <f>IF(A122="","","/* ") &amp; "`" &amp; C122 &amp; "` " &amp; D122 &amp; IF(E122&gt;0,"(" &amp; E122 &amp; ") "," ") &amp; IF(F122&lt;&gt;"","NOT NULL ","") &amp; IF(G122="","","DEFAULT '" &amp; G122 &amp; "' ") &amp; "COMMENT '"&amp; B122 &amp;"'," &amp; IF(A122="",""," */")</f>
+        <v>`timelogcategory_id` INT COMMENT 'カテゴリ',</v>
+      </c>
+      <c r="J122" s="36" t="str">
+        <f t="shared" ref="J122:J127" si="31">"," &amp;  "`" &amp; C122 &amp; "` " &amp; D122 &amp; IF(E122&gt;0,"(" &amp; E122 &amp; ") "," ") &amp; IF(F122&lt;&gt;"","NOT NULL ","") &amp; IF(G122="","","DEFAULT '" &amp; G122 &amp; "' ")</f>
+        <v xml:space="preserve">,`timelogcategory_id` INT </v>
+      </c>
     </row>
     <row r="123" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="B123" s="51" t="s">
-        <v>106</v>
-      </c>
-      <c r="C123" s="51" t="s">
-        <v>107</v>
-      </c>
-      <c r="D123" s="33"/>
-      <c r="E123" s="34"/>
-      <c r="F123" s="34"/>
-      <c r="G123" s="34"/>
-      <c r="H123" s="35"/>
-      <c r="I123" s="27" t="str">
-        <f xml:space="preserve"> "CREATE TABLE `" &amp; C123 &amp; "` ("</f>
-        <v>CREATE TABLE `timelogtasks` (</v>
-      </c>
-      <c r="J123" s="27" t="str">
-        <f xml:space="preserve"> "CREATE TABLE `" &amp; C123 &amp; "` ("</f>
-        <v>CREATE TABLE `timelogtasks` (</v>
+      <c r="B123" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="C123" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="D123" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="E123" s="16"/>
+      <c r="F123" s="16"/>
+      <c r="G123" s="16"/>
+      <c r="H123" s="17"/>
+      <c r="I123" s="36" t="str">
+        <f>IF(A123="","","/* ") &amp; "`" &amp; C123 &amp; "` " &amp; D123 &amp; IF(E123&gt;0,"(" &amp; E123 &amp; ") "," ") &amp; IF(F123&lt;&gt;"","NOT NULL ","") &amp; IF(G123="","","DEFAULT '" &amp; G123 &amp; "' ") &amp; "COMMENT '"&amp; B123 &amp;"'," &amp; IF(A123="",""," */")</f>
+        <v>`timelogtask_id` INT COMMENT 'タスク',</v>
+      </c>
+      <c r="J123" s="36" t="str">
+        <f t="shared" ref="J123" si="32">"," &amp;  "`" &amp; C123 &amp; "` " &amp; D123 &amp; IF(E123&gt;0,"(" &amp; E123 &amp; ") "," ") &amp; IF(F123&lt;&gt;"","NOT NULL ","") &amp; IF(G123="","","DEFAULT '" &amp; G123 &amp; "' ")</f>
+        <v xml:space="preserve">,`timelogtask_id` INT </v>
       </c>
     </row>
     <row r="124" spans="1:10" x14ac:dyDescent="0.15">
       <c r="B124" s="15" t="s">
-        <v>9</v>
+        <v>70</v>
       </c>
       <c r="C124" s="15" t="s">
-        <v>1</v>
+        <v>102</v>
       </c>
       <c r="D124" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="E124" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="F124" s="16"/>
+        <v>73</v>
+      </c>
+      <c r="E124" s="16"/>
+      <c r="F124" s="16" t="s">
+        <v>72</v>
+      </c>
       <c r="G124" s="16"/>
       <c r="H124" s="17"/>
-      <c r="I124" s="27" t="s">
-        <v>3</v>
-      </c>
-      <c r="J124" s="27" t="s">
-        <v>87</v>
+      <c r="I124" s="36" t="str">
+        <f t="shared" ref="I124:I126" si="33">IF(A124="","","/* ") &amp; "`" &amp; C124 &amp; "` " &amp; D124 &amp; IF(E124&gt;0,"(" &amp; E124 &amp; ") "," ") &amp; IF(F124&lt;&gt;"","NOT NULL ","") &amp; IF(G124="","","DEFAULT '" &amp; G124 &amp; "' ") &amp; "COMMENT '"&amp; B124 &amp;"'," &amp; IF(A124="",""," */")</f>
+        <v>`workdate` DATE NOT NULL COMMENT '日付',</v>
+      </c>
+      <c r="J124" s="36" t="str">
+        <f t="shared" si="31"/>
+        <v xml:space="preserve">,`workdate` DATE NOT NULL </v>
       </c>
     </row>
     <row r="125" spans="1:10" x14ac:dyDescent="0.15">
       <c r="B125" s="15" t="s">
-        <v>15</v>
+        <v>109</v>
       </c>
       <c r="C125" s="15" t="s">
-        <v>12</v>
+        <v>110</v>
       </c>
       <c r="D125" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="E125" s="16">
-        <v>128</v>
+        <v>111</v>
+      </c>
+      <c r="E125" s="16" t="s">
+        <v>112</v>
       </c>
       <c r="F125" s="16" t="s">
         <v>7</v>
@@ -4550,39 +4678,37 @@
       <c r="G125" s="16"/>
       <c r="H125" s="17"/>
       <c r="I125" s="36" t="str">
-        <f t="shared" ref="I125" si="37">IF(A125="","","/* ") &amp; "`" &amp; C125 &amp; "` " &amp; D125 &amp; IF(E125&gt;0,"(" &amp; E125 &amp; ") "," ") &amp; IF(F125&lt;&gt;"","NOT NULL ","") &amp; IF(G125="","","DEFAULT '" &amp; G125 &amp; "' ") &amp; "COMMENT '"&amp; B125 &amp;"'," &amp; IF(A125="",""," */")</f>
-        <v>`name` VARCHAR(128) NOT NULL COMMENT '名前',</v>
+        <f t="shared" ref="I125" si="34">IF(A125="","","/* ") &amp; "`" &amp; C125 &amp; "` " &amp; D125 &amp; IF(E125&gt;0,"(" &amp; E125 &amp; ") "," ") &amp; IF(F125&lt;&gt;"","NOT NULL ","") &amp; IF(G125="","","DEFAULT '" &amp; G125 &amp; "' ") &amp; "COMMENT '"&amp; B125 &amp;"'," &amp; IF(A125="",""," */")</f>
+        <v>`worktime` DECIMAL(5,2) NOT NULL COMMENT '時間',</v>
       </c>
       <c r="J125" s="36" t="str">
-        <f t="shared" ref="J125:J129" si="38">"," &amp;  "`" &amp; C125 &amp; "` " &amp; D125 &amp; IF(E125&gt;0,"(" &amp; E125 &amp; ") "," ") &amp; IF(F125&lt;&gt;"","NOT NULL ","") &amp; IF(G125="","","DEFAULT '" &amp; G125 &amp; "' ")</f>
-        <v xml:space="preserve">,`name` VARCHAR(128) NOT NULL </v>
+        <f t="shared" ref="J125" si="35">"," &amp;  "`" &amp; C125 &amp; "` " &amp; D125 &amp; IF(E125&gt;0,"(" &amp; E125 &amp; ") "," ") &amp; IF(F125&lt;&gt;"","NOT NULL ","") &amp; IF(G125="","","DEFAULT '" &amp; G125 &amp; "' ")</f>
+        <v xml:space="preserve">,`worktime` DECIMAL(5,2) NOT NULL </v>
       </c>
     </row>
     <row r="126" spans="1:10" x14ac:dyDescent="0.15">
       <c r="B126" s="15" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="C126" s="15" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D126" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="E126" s="16"/>
-      <c r="F126" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="G126" s="16">
-        <v>0</v>
-      </c>
+        <v>103</v>
+      </c>
+      <c r="E126" s="16">
+        <v>256</v>
+      </c>
+      <c r="F126" s="16"/>
+      <c r="G126" s="16"/>
       <c r="H126" s="17"/>
       <c r="I126" s="36" t="str">
-        <f>IF(A126="","","/* ") &amp; "`" &amp; C126 &amp; "` " &amp; D126 &amp; IF(E126&gt;0,"(" &amp; E126 &amp; ") "," ") &amp; IF(F126&lt;&gt;"","NOT NULL ","") &amp; IF(G126="","","DEFAULT '" &amp; G126 &amp; "' ") &amp; "COMMENT '"&amp; B126 &amp;"'," &amp; IF(A126="",""," */")</f>
-        <v>`position` INT NOT NULL DEFAULT '0' COMMENT 'position',</v>
+        <f t="shared" si="33"/>
+        <v>`title` VARCHAR(256) COMMENT '名前',</v>
       </c>
       <c r="J126" s="36" t="str">
-        <f t="shared" si="38"/>
-        <v xml:space="preserve">,`position` INT NOT NULL DEFAULT '0' </v>
+        <f t="shared" si="31"/>
+        <v xml:space="preserve">,`title` VARCHAR(256) </v>
       </c>
     </row>
     <row r="127" spans="1:10" x14ac:dyDescent="0.15">
@@ -4601,504 +4727,718 @@
       <c r="G127" s="16"/>
       <c r="H127" s="17"/>
       <c r="I127" s="36" t="str">
-        <f t="shared" ref="I127:I129" si="39">IF(A127="","","/* ") &amp; "`" &amp; C127 &amp; "` " &amp; D127 &amp; IF(E127&gt;0,"(" &amp; E127 &amp; ") "," ") &amp; IF(F127&lt;&gt;"","NOT NULL ","") &amp; IF(G127="","","DEFAULT '" &amp; G127 &amp; "' ") &amp; "COMMENT '"&amp; B127 &amp;"'," &amp; IF(A127="",""," */")</f>
+        <f t="shared" ref="I127" si="36">IF(A127="","","/* ") &amp; "`" &amp; C127 &amp; "` " &amp; D127 &amp; IF(E127&gt;0,"(" &amp; E127 &amp; ") "," ") &amp; IF(F127&lt;&gt;"","NOT NULL ","") &amp; IF(G127="","","DEFAULT '" &amp; G127 &amp; "' ") &amp; "COMMENT '"&amp; B127 &amp;"'," &amp; IF(A127="",""," */")</f>
         <v>`created` DATETIME COMMENT '登録日',</v>
       </c>
       <c r="J127" s="36" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="31"/>
         <v xml:space="preserve">,`created` DATETIME </v>
       </c>
     </row>
     <row r="128" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A128" s="22"/>
       <c r="B128" s="15" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="C128" s="18" t="s">
-        <v>89</v>
+        <v>105</v>
       </c>
       <c r="D128" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="E128" s="16">
-        <v>4</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="E128" s="16"/>
       <c r="F128" s="16"/>
-      <c r="G128" s="16">
-        <v>0</v>
-      </c>
+      <c r="G128" s="16"/>
       <c r="H128" s="17"/>
       <c r="I128" s="36" t="str">
-        <f t="shared" si="39"/>
-        <v>`deleted` TINYINT(4) DEFAULT '0' COMMENT '削除フラグ',</v>
+        <f t="shared" ref="I128" si="37">IF(A128="","","/* ") &amp; "`" &amp; C128 &amp; "` " &amp; D128 &amp; IF(E128&gt;0,"(" &amp; E128 &amp; ") "," ") &amp; IF(F128&lt;&gt;"","NOT NULL ","") &amp; IF(G128="","","DEFAULT '" &amp; G128 &amp; "' ") &amp; "COMMENT '"&amp; B128 &amp;"'," &amp; IF(A128="",""," */")</f>
+        <v>`modified` DATETIME COMMENT '変更日',</v>
       </c>
       <c r="J128" s="36" t="str">
-        <f t="shared" si="38"/>
-        <v xml:space="preserve">,`deleted` TINYINT(4) DEFAULT '0' </v>
+        <f t="shared" ref="J128" si="38">"," &amp;  "`" &amp; C128 &amp; "` " &amp; D128 &amp; IF(E128&gt;0,"(" &amp; E128 &amp; ") "," ") &amp; IF(F128&lt;&gt;"","NOT NULL ","") &amp; IF(G128="","","DEFAULT '" &amp; G128 &amp; "' ")</f>
+        <v xml:space="preserve">,`modified` DATETIME </v>
       </c>
     </row>
     <row r="129" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A129" s="22"/>
-      <c r="B129" s="15" t="s">
+      <c r="I129" s="37" t="s">
+        <v>2</v>
+      </c>
+      <c r="J129" s="37" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="130" spans="1:10" s="28" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="A130" s="43"/>
+      <c r="H130" s="29"/>
+    </row>
+    <row r="131" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="B131" s="42"/>
+      <c r="D131" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="E131" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="F131" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="G131" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="H131" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="I131" s="30"/>
+      <c r="J131" s="30"/>
+    </row>
+    <row r="132" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="B132" s="51" t="s">
+        <v>106</v>
+      </c>
+      <c r="C132" s="51" t="s">
+        <v>107</v>
+      </c>
+      <c r="D132" s="33"/>
+      <c r="E132" s="34"/>
+      <c r="F132" s="34"/>
+      <c r="G132" s="34"/>
+      <c r="H132" s="35"/>
+      <c r="I132" s="27" t="str">
+        <f xml:space="preserve"> "CREATE TABLE `" &amp; C132 &amp; "` ("</f>
+        <v>CREATE TABLE `timelogtasks` (</v>
+      </c>
+      <c r="J132" s="27" t="str">
+        <f xml:space="preserve"> "CREATE TABLE `" &amp; C132 &amp; "` ("</f>
+        <v>CREATE TABLE `timelogtasks` (</v>
+      </c>
+    </row>
+    <row r="133" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="B133" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C133" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="D133" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E133" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F133" s="16"/>
+      <c r="G133" s="16"/>
+      <c r="H133" s="17"/>
+      <c r="I133" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="J133" s="27" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="134" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="B134" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C134" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D134" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E134" s="16">
+        <v>128</v>
+      </c>
+      <c r="F134" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="G134" s="16"/>
+      <c r="H134" s="17"/>
+      <c r="I134" s="36" t="str">
+        <f t="shared" ref="I134" si="39">IF(A134="","","/* ") &amp; "`" &amp; C134 &amp; "` " &amp; D134 &amp; IF(E134&gt;0,"(" &amp; E134 &amp; ") "," ") &amp; IF(F134&lt;&gt;"","NOT NULL ","") &amp; IF(G134="","","DEFAULT '" &amp; G134 &amp; "' ") &amp; "COMMENT '"&amp; B134 &amp;"'," &amp; IF(A134="",""," */")</f>
+        <v>`name` VARCHAR(128) NOT NULL COMMENT '名前',</v>
+      </c>
+      <c r="J134" s="36" t="str">
+        <f t="shared" ref="J134:J138" si="40">"," &amp;  "`" &amp; C134 &amp; "` " &amp; D134 &amp; IF(E134&gt;0,"(" &amp; E134 &amp; ") "," ") &amp; IF(F134&lt;&gt;"","NOT NULL ","") &amp; IF(G134="","","DEFAULT '" &amp; G134 &amp; "' ")</f>
+        <v xml:space="preserve">,`name` VARCHAR(128) NOT NULL </v>
+      </c>
+    </row>
+    <row r="135" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="B135" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C135" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="D135" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="E135" s="16"/>
+      <c r="F135" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="G135" s="16">
+        <v>0</v>
+      </c>
+      <c r="H135" s="17"/>
+      <c r="I135" s="36" t="str">
+        <f>IF(A135="","","/* ") &amp; "`" &amp; C135 &amp; "` " &amp; D135 &amp; IF(E135&gt;0,"(" &amp; E135 &amp; ") "," ") &amp; IF(F135&lt;&gt;"","NOT NULL ","") &amp; IF(G135="","","DEFAULT '" &amp; G135 &amp; "' ") &amp; "COMMENT '"&amp; B135 &amp;"'," &amp; IF(A135="",""," */")</f>
+        <v>`position` INT NOT NULL DEFAULT '0' COMMENT 'position',</v>
+      </c>
+      <c r="J135" s="36" t="str">
+        <f t="shared" si="40"/>
+        <v xml:space="preserve">,`position` INT NOT NULL DEFAULT '0' </v>
+      </c>
+    </row>
+    <row r="136" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A136" s="22"/>
+      <c r="B136" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C136" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="D136" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E136" s="16"/>
+      <c r="F136" s="16"/>
+      <c r="G136" s="16"/>
+      <c r="H136" s="17"/>
+      <c r="I136" s="36" t="str">
+        <f t="shared" ref="I136:I138" si="41">IF(A136="","","/* ") &amp; "`" &amp; C136 &amp; "` " &amp; D136 &amp; IF(E136&gt;0,"(" &amp; E136 &amp; ") "," ") &amp; IF(F136&lt;&gt;"","NOT NULL ","") &amp; IF(G136="","","DEFAULT '" &amp; G136 &amp; "' ") &amp; "COMMENT '"&amp; B136 &amp;"'," &amp; IF(A136="",""," */")</f>
+        <v>`created` DATETIME COMMENT '登録日',</v>
+      </c>
+      <c r="J136" s="36" t="str">
+        <f t="shared" si="40"/>
+        <v xml:space="preserve">,`created` DATETIME </v>
+      </c>
+    </row>
+    <row r="137" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A137" s="22"/>
+      <c r="B137" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="C137" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="D137" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="E137" s="16">
+        <v>4</v>
+      </c>
+      <c r="F137" s="16"/>
+      <c r="G137" s="16">
+        <v>0</v>
+      </c>
+      <c r="H137" s="17"/>
+      <c r="I137" s="36" t="str">
+        <f t="shared" si="41"/>
+        <v>`deleted` TINYINT(4) DEFAULT '0' COMMENT '削除フラグ',</v>
+      </c>
+      <c r="J137" s="36" t="str">
+        <f t="shared" si="40"/>
+        <v xml:space="preserve">,`deleted` TINYINT(4) DEFAULT '0' </v>
+      </c>
+    </row>
+    <row r="138" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A138" s="22"/>
+      <c r="B138" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="C129" s="18" t="s">
+      <c r="C138" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="D129" s="15" t="s">
+      <c r="D138" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="E129" s="16"/>
-      <c r="F129" s="16"/>
-      <c r="G129" s="16"/>
-      <c r="H129" s="17"/>
-      <c r="I129" s="36" t="str">
-        <f t="shared" si="39"/>
+      <c r="E138" s="16"/>
+      <c r="F138" s="16"/>
+      <c r="G138" s="16"/>
+      <c r="H138" s="17"/>
+      <c r="I138" s="36" t="str">
+        <f t="shared" si="41"/>
         <v>`deleted_date` DATETIME COMMENT '削除日',</v>
       </c>
-      <c r="J129" s="36" t="str">
-        <f t="shared" si="38"/>
+      <c r="J138" s="36" t="str">
+        <f t="shared" si="40"/>
         <v xml:space="preserve">,`deleted_date` DATETIME </v>
       </c>
     </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A130" s="22"/>
-      <c r="I130" s="37" t="s">
+    <row r="139" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A139" s="22"/>
+      <c r="I139" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="J130" s="37" t="s">
+      <c r="J139" s="37" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="131" spans="1:10" s="28" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="A131" s="43"/>
-      <c r="H131" s="29"/>
+    <row r="140" spans="1:10" s="28" customFormat="1" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="A140" s="43"/>
+      <c r="H140" s="29"/>
     </row>
   </sheetData>
   <phoneticPr fontId="7"/>
-  <conditionalFormatting sqref="B1:B3 B17 B24 B13 B35 B74:B75 B132:B1048576">
-    <cfRule type="expression" dxfId="86" priority="241">
+  <conditionalFormatting sqref="B1:B3 B17 B24 B13 B35 B74:B75 B141:B1048576">
+    <cfRule type="expression" dxfId="91" priority="249">
       <formula>A1&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B21:B23">
-    <cfRule type="expression" dxfId="85" priority="112">
+    <cfRule type="expression" dxfId="90" priority="120">
       <formula>A21&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14:B16">
-    <cfRule type="expression" dxfId="84" priority="111">
+    <cfRule type="expression" dxfId="89" priority="119">
       <formula>A14&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19">
-    <cfRule type="expression" dxfId="83" priority="110">
+    <cfRule type="expression" dxfId="88" priority="118">
       <formula>A19&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12">
+    <cfRule type="expression" dxfId="87" priority="116">
+      <formula>A12&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B4:B7">
+    <cfRule type="expression" dxfId="86" priority="115">
+      <formula>A4&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B9">
+    <cfRule type="expression" dxfId="85" priority="113">
+      <formula>A9&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B18">
+    <cfRule type="expression" dxfId="84" priority="112">
+      <formula>A18&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B8">
+    <cfRule type="expression" dxfId="83" priority="111">
+      <formula>A8&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B25:B26">
     <cfRule type="expression" dxfId="82" priority="108">
-      <formula>A12&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B4:B7">
-    <cfRule type="expression" dxfId="81" priority="107">
-      <formula>A4&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B9">
-    <cfRule type="expression" dxfId="80" priority="105">
-      <formula>A9&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B18">
-    <cfRule type="expression" dxfId="79" priority="104">
-      <formula>A18&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B8">
-    <cfRule type="expression" dxfId="78" priority="103">
-      <formula>A8&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B25:B26">
-    <cfRule type="expression" dxfId="77" priority="100">
       <formula>A25&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20">
-    <cfRule type="expression" dxfId="76" priority="97">
+    <cfRule type="expression" dxfId="81" priority="105">
       <formula>A20&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B28">
-    <cfRule type="expression" dxfId="75" priority="96">
+    <cfRule type="expression" dxfId="80" priority="104">
       <formula>A28&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B32:B34">
-    <cfRule type="expression" dxfId="74" priority="95">
+    <cfRule type="expression" dxfId="79" priority="103">
       <formula>A32&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B27">
-    <cfRule type="expression" dxfId="73" priority="94">
+    <cfRule type="expression" dxfId="78" priority="102">
       <formula>A27&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B30">
-    <cfRule type="expression" dxfId="72" priority="93">
+    <cfRule type="expression" dxfId="77" priority="101">
       <formula>A30&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B29">
-    <cfRule type="expression" dxfId="71" priority="92">
+    <cfRule type="expression" dxfId="76" priority="100">
       <formula>A29&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B31">
-    <cfRule type="expression" dxfId="70" priority="91">
+    <cfRule type="expression" dxfId="75" priority="99">
       <formula>A31&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B45 B56">
-    <cfRule type="expression" dxfId="69" priority="79">
+    <cfRule type="expression" dxfId="74" priority="87">
       <formula>A45&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B44">
-    <cfRule type="expression" dxfId="68" priority="78">
+    <cfRule type="expression" dxfId="73" priority="86">
       <formula>A44&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B38:B39">
-    <cfRule type="expression" dxfId="67" priority="77">
+    <cfRule type="expression" dxfId="72" priority="85">
       <formula>A38&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B40">
-    <cfRule type="expression" dxfId="66" priority="76">
+    <cfRule type="expression" dxfId="71" priority="84">
       <formula>A40&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B37">
-    <cfRule type="expression" dxfId="65" priority="75">
+    <cfRule type="expression" dxfId="70" priority="83">
       <formula>A37&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B41">
-    <cfRule type="expression" dxfId="64" priority="74">
+    <cfRule type="expression" dxfId="69" priority="82">
       <formula>A41&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B36">
-    <cfRule type="expression" dxfId="63" priority="73">
+    <cfRule type="expression" dxfId="68" priority="81">
       <formula>A36&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B54:B55">
-    <cfRule type="expression" dxfId="62" priority="72">
+    <cfRule type="expression" dxfId="67" priority="80">
       <formula>A54&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B46 B50:B52 B48">
-    <cfRule type="expression" dxfId="61" priority="71">
+    <cfRule type="expression" dxfId="66" priority="79">
       <formula>A46&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B53">
-    <cfRule type="expression" dxfId="60" priority="70">
+    <cfRule type="expression" dxfId="65" priority="78">
       <formula>A53&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B49">
-    <cfRule type="expression" dxfId="59" priority="69">
+    <cfRule type="expression" dxfId="64" priority="77">
       <formula>A49&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B47">
-    <cfRule type="expression" dxfId="58" priority="68">
+    <cfRule type="expression" dxfId="63" priority="76">
       <formula>A47&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B72 B76 B66">
-    <cfRule type="expression" dxfId="57" priority="67">
+    <cfRule type="expression" dxfId="62" priority="75">
       <formula>A66&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B67:B69">
-    <cfRule type="expression" dxfId="56" priority="65">
+    <cfRule type="expression" dxfId="61" priority="73">
       <formula>A67&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B65">
-    <cfRule type="expression" dxfId="55" priority="63">
+    <cfRule type="expression" dxfId="60" priority="71">
       <formula>A65&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B57:B60">
-    <cfRule type="expression" dxfId="54" priority="62">
+    <cfRule type="expression" dxfId="59" priority="70">
       <formula>A57&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B62">
-    <cfRule type="expression" dxfId="53" priority="61">
+    <cfRule type="expression" dxfId="58" priority="69">
       <formula>A62&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B70">
-    <cfRule type="expression" dxfId="52" priority="60">
+    <cfRule type="expression" dxfId="57" priority="68">
       <formula>A70&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B61">
-    <cfRule type="expression" dxfId="51" priority="59">
+    <cfRule type="expression" dxfId="56" priority="67">
       <formula>A61&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B73">
-    <cfRule type="expression" dxfId="50" priority="58">
+    <cfRule type="expression" dxfId="55" priority="66">
       <formula>A73&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B71">
-    <cfRule type="expression" dxfId="49" priority="57">
+    <cfRule type="expression" dxfId="54" priority="65">
       <formula>A71&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B88">
-    <cfRule type="expression" dxfId="48" priority="51">
+    <cfRule type="expression" dxfId="53" priority="59">
       <formula>A88&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B81 B79">
-    <cfRule type="expression" dxfId="47" priority="50">
+    <cfRule type="expression" dxfId="52" priority="58">
       <formula>A79&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B89">
-    <cfRule type="expression" dxfId="46" priority="49">
+    <cfRule type="expression" dxfId="51" priority="57">
       <formula>A89&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B82">
-    <cfRule type="expression" dxfId="45" priority="48">
+    <cfRule type="expression" dxfId="50" priority="56">
       <formula>A82&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B87">
-    <cfRule type="expression" dxfId="44" priority="47">
+    <cfRule type="expression" dxfId="49" priority="55">
       <formula>A87&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B85">
+    <cfRule type="expression" dxfId="48" priority="54">
+      <formula>A85&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B83">
+    <cfRule type="expression" dxfId="47" priority="53">
+      <formula>A83&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B86">
+    <cfRule type="expression" dxfId="46" priority="52">
+      <formula>A86&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B80">
+    <cfRule type="expression" dxfId="45" priority="51">
+      <formula>A80&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B84">
+    <cfRule type="expression" dxfId="44" priority="50">
+      <formula>A84&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B77">
     <cfRule type="expression" dxfId="43" priority="46">
-      <formula>A85&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B83">
-    <cfRule type="expression" dxfId="42" priority="45">
-      <formula>A83&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B86">
-    <cfRule type="expression" dxfId="41" priority="44">
-      <formula>A86&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B80">
-    <cfRule type="expression" dxfId="40" priority="43">
-      <formula>A80&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B84">
-    <cfRule type="expression" dxfId="39" priority="42">
-      <formula>A84&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B77">
-    <cfRule type="expression" dxfId="38" priority="38">
       <formula>A77&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B78">
-    <cfRule type="expression" dxfId="37" priority="39">
+    <cfRule type="expression" dxfId="42" priority="47">
       <formula>A78&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B98">
-    <cfRule type="expression" dxfId="36" priority="37">
+    <cfRule type="expression" dxfId="41" priority="45">
       <formula>A98&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B90 B92:B93">
-    <cfRule type="expression" dxfId="35" priority="36">
+    <cfRule type="expression" dxfId="40" priority="44">
       <formula>A90&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B99">
-    <cfRule type="expression" dxfId="34" priority="35">
+    <cfRule type="expression" dxfId="39" priority="43">
       <formula>A99&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B94">
-    <cfRule type="expression" dxfId="33" priority="34">
+    <cfRule type="expression" dxfId="38" priority="42">
       <formula>A94&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B95">
-    <cfRule type="expression" dxfId="32" priority="33">
+    <cfRule type="expression" dxfId="37" priority="41">
       <formula>A95&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B91">
-    <cfRule type="expression" dxfId="31" priority="31">
+    <cfRule type="expression" dxfId="36" priority="39">
       <formula>A91&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10">
-    <cfRule type="expression" dxfId="30" priority="30">
+    <cfRule type="expression" dxfId="35" priority="38">
       <formula>A10&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B11">
-    <cfRule type="expression" dxfId="29" priority="29">
+    <cfRule type="expression" dxfId="34" priority="37">
       <formula>A11&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B42">
-    <cfRule type="expression" dxfId="28" priority="28">
+    <cfRule type="expression" dxfId="33" priority="36">
       <formula>A42&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B43">
-    <cfRule type="expression" dxfId="27" priority="27">
+    <cfRule type="expression" dxfId="32" priority="35">
       <formula>A43&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B63">
-    <cfRule type="expression" dxfId="26" priority="26">
+    <cfRule type="expression" dxfId="31" priority="34">
       <formula>A63&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B64">
-    <cfRule type="expression" dxfId="25" priority="25">
+    <cfRule type="expression" dxfId="30" priority="33">
       <formula>A64&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B96">
-    <cfRule type="expression" dxfId="24" priority="24">
+    <cfRule type="expression" dxfId="29" priority="32">
       <formula>A96&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B97">
-    <cfRule type="expression" dxfId="23" priority="23">
+    <cfRule type="expression" dxfId="28" priority="31">
       <formula>A97&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="B116">
+    <cfRule type="expression" dxfId="27" priority="19">
+      <formula>A116&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B127 B129">
+    <cfRule type="expression" dxfId="26" priority="30">
+      <formula>A127&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B126 B130 B118">
+    <cfRule type="expression" dxfId="25" priority="29">
+      <formula>A118&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B119:B121">
+    <cfRule type="expression" dxfId="24" priority="28">
+      <formula>A119&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B117">
+    <cfRule type="expression" dxfId="23" priority="27">
+      <formula>A117&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B109:B112">
+    <cfRule type="expression" dxfId="22" priority="26">
+      <formula>A109&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B114">
+    <cfRule type="expression" dxfId="21" priority="25">
+      <formula>A114&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B122">
+    <cfRule type="expression" dxfId="20" priority="24">
+      <formula>A122&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B113">
+    <cfRule type="expression" dxfId="19" priority="23">
+      <formula>A113&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B124">
+    <cfRule type="expression" dxfId="18" priority="21">
+      <formula>A124&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B115">
+    <cfRule type="expression" dxfId="17" priority="20">
+      <formula>A115&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B138">
+    <cfRule type="expression" dxfId="16" priority="12">
+      <formula>A138&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B140">
+    <cfRule type="expression" dxfId="15" priority="18">
+      <formula>A140&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B139">
+    <cfRule type="expression" dxfId="14" priority="17">
+      <formula>A139&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B131:B134">
+    <cfRule type="expression" dxfId="13" priority="16">
+      <formula>A131&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B136">
+    <cfRule type="expression" dxfId="12" priority="15">
+      <formula>A136&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B135">
+    <cfRule type="expression" dxfId="11" priority="14">
+      <formula>A135&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B137">
+    <cfRule type="expression" dxfId="10" priority="13">
+      <formula>A137&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B123">
+    <cfRule type="expression" dxfId="9" priority="11">
+      <formula>A123&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B128">
+    <cfRule type="expression" dxfId="8" priority="10">
+      <formula>A128&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B125">
+    <cfRule type="expression" dxfId="7" priority="9">
+      <formula>A125&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="B107">
-    <cfRule type="expression" dxfId="22" priority="11">
+    <cfRule type="expression" dxfId="6" priority="8">
       <formula>A107&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B118 B120">
-    <cfRule type="expression" dxfId="21" priority="22">
-      <formula>A118&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B117 B121 B109">
-    <cfRule type="expression" dxfId="20" priority="21">
-      <formula>A109&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B110:B112">
-    <cfRule type="expression" dxfId="19" priority="20">
-      <formula>A110&lt;&gt;""</formula>
+  <conditionalFormatting sqref="B100 B102:B103">
+    <cfRule type="expression" dxfId="5" priority="7">
+      <formula>A100&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B108">
-    <cfRule type="expression" dxfId="18" priority="19">
+    <cfRule type="expression" dxfId="4" priority="6">
       <formula>A108&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B100:B103">
-    <cfRule type="expression" dxfId="17" priority="18">
-      <formula>A100&lt;&gt;""</formula>
+  <conditionalFormatting sqref="B104">
+    <cfRule type="expression" dxfId="3" priority="5">
+      <formula>A104&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B105">
-    <cfRule type="expression" dxfId="16" priority="17">
+    <cfRule type="expression" dxfId="2" priority="4">
       <formula>A105&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B113">
-    <cfRule type="expression" dxfId="15" priority="16">
-      <formula>A113&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B104">
-    <cfRule type="expression" dxfId="14" priority="15">
-      <formula>A104&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B115">
-    <cfRule type="expression" dxfId="13" priority="13">
-      <formula>A115&lt;&gt;""</formula>
+  <conditionalFormatting sqref="B101">
+    <cfRule type="expression" dxfId="1" priority="3">
+      <formula>A101&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B106">
-    <cfRule type="expression" dxfId="12" priority="12">
+    <cfRule type="expression" dxfId="0" priority="2">
       <formula>A106&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B129">
-    <cfRule type="expression" dxfId="11" priority="4">
-      <formula>A129&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B131">
-    <cfRule type="expression" dxfId="10" priority="10">
-      <formula>A131&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B130">
-    <cfRule type="expression" dxfId="9" priority="9">
-      <formula>A130&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B122:B125">
-    <cfRule type="expression" dxfId="8" priority="8">
-      <formula>A122&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B127">
-    <cfRule type="expression" dxfId="7" priority="7">
-      <formula>A127&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B126">
-    <cfRule type="expression" dxfId="6" priority="6">
-      <formula>A126&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B128">
-    <cfRule type="expression" dxfId="5" priority="5">
-      <formula>A128&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B114">
-    <cfRule type="expression" dxfId="4" priority="3">
-      <formula>A114&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B119">
-    <cfRule type="expression" dxfId="3" priority="2">
-      <formula>A119&lt;&gt;""</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B116">
-    <cfRule type="expression" dxfId="2" priority="1">
-      <formula>A116&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>